<commit_message>
adding my review comments on HLD in design doc peer review sheet
</commit_message>
<xml_diff>
--- a/Design/Design document Peer Review sheet.xlsx
+++ b/Design/Design document Peer Review sheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\iti\project managment\design 2\Internet-Banking-System\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>Priority</t>
   </si>
@@ -84,13 +84,72 @@
   </si>
   <si>
     <t xml:space="preserve"> Date</t>
+  </si>
+  <si>
+    <t>1-</t>
+  </si>
+  <si>
+    <t>missing in( C)(2) to check balance before transferring money to an account in the same bank</t>
+  </si>
+  <si>
+    <t>2-</t>
+  </si>
+  <si>
+    <t>3-</t>
+  </si>
+  <si>
+    <t>4-</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Bank_SYS_HLD_client_005
+Bank_SYS_HLD_admin_005</t>
+  </si>
+  <si>
+    <t>Bank_SYS_HLD_client_006
+Bank_SYS_HLD_admin_006</t>
+  </si>
+  <si>
+    <t>missing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">missing </t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Admin_R007</t>
+  </si>
+  <si>
+    <t>missing that the admin can make request to view an account balance .</t>
+  </si>
+  <si>
+    <t>missing that the admin can make request to view the account previous transactions.</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_TR_R008</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_TR_R008
+BANK_SYS_SRS_TR_R027</t>
+  </si>
+  <si>
+    <t>after adding check balance request , we need to  
+to elaborate response in two cases 
+1- customer balance covers transaction&amp; doesn't exceed the amount he can transfer to aspecific account.
+2- customer balance is greater than transaction ot 
+ exceeds the amount he can transfer to aspecific account.</t>
+  </si>
+  <si>
+    <t>missing to elaborate the response in case customer wants to  transfer amount of money greater than his balance to other bank or exceeds the amount he can transfer to a specific account 
+ after (D)(3)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -157,6 +216,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -172,7 +237,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="44">
+  <borders count="45">
     <border>
       <left/>
       <right/>
@@ -729,6 +794,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -736,7 +814,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -854,9 +932,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -988,6 +1063,12 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1590,7 +1671,7 @@
   <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1608,15 +1689,15 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15" thickBot="1"/>
     <row r="2" spans="1:8" ht="105" customHeight="1" thickBot="1">
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="74"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="73"/>
     </row>
     <row r="3" spans="1:8" ht="14.25" customHeight="1">
       <c r="C3" s="7"/>
@@ -1633,68 +1714,68 @@
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:8" ht="20.25" customHeight="1">
-      <c r="C5" s="81" t="s">
+      <c r="C5" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="81" t="s">
+      <c r="D5" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="81" t="s">
+      <c r="E5" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="81" t="s">
+      <c r="F5" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="81" t="s">
+      <c r="G5" s="80" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="23.25" customHeight="1" thickBot="1">
-      <c r="C6" s="82"/>
-      <c r="D6" s="82"/>
-      <c r="E6" s="83"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="82"/>
+      <c r="C6" s="81"/>
+      <c r="D6" s="81"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="81"/>
+      <c r="G6" s="81"/>
     </row>
     <row r="7" spans="1:8" ht="29.25" customHeight="1">
       <c r="C7" s="12">
         <v>1</v>
       </c>
-      <c r="D7" s="63" t="s">
+      <c r="D7" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="62">
+      <c r="E7" s="61">
         <v>43713</v>
       </c>
-      <c r="F7" s="59"/>
+      <c r="F7" s="58"/>
       <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:8" ht="21.75" customHeight="1">
-      <c r="C8" s="54"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="60"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="59"/>
       <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:8" ht="21.75" customHeight="1">
-      <c r="C9" s="54"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="60"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="59"/>
       <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:8" ht="21.75" customHeight="1">
-      <c r="C10" s="54"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="60"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="59"/>
       <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:8" ht="20.25" customHeight="1">
-      <c r="C11" s="54"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="60"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="59"/>
       <c r="G11" s="9"/>
     </row>
     <row r="12" spans="1:8" ht="14.25" customHeight="1">
@@ -1753,73 +1834,115 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="56.25" customHeight="1" thickTop="1">
+    <row r="17" spans="1:8" ht="139.5" customHeight="1" thickTop="1">
       <c r="A17" s="21"/>
-      <c r="B17" s="75" t="s">
+      <c r="B17" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="39"/>
-    </row>
-    <row r="18" spans="1:8" ht="57" customHeight="1">
+      <c r="C17" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" s="83" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="57" customHeight="1" thickBot="1">
       <c r="A18" s="21"/>
-      <c r="B18" s="70"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="4"/>
+      <c r="B18" s="69"/>
+      <c r="C18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="84" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="H18" s="13"/>
     </row>
     <row r="19" spans="1:8" ht="54.75" customHeight="1">
       <c r="A19" s="21"/>
-      <c r="B19" s="70"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="4"/>
+      <c r="B19" s="69"/>
+      <c r="C19" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="H19" s="13"/>
     </row>
-    <row r="20" spans="1:8" s="1" customFormat="1" ht="54" customHeight="1" thickBot="1">
+    <row r="20" spans="1:8" s="1" customFormat="1" ht="72.75" customHeight="1" thickBot="1">
       <c r="A20" s="22"/>
-      <c r="B20" s="76"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="33"/>
+      <c r="B20" s="75"/>
+      <c r="C20" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="G20" s="33" t="s">
+        <v>24</v>
+      </c>
       <c r="H20" s="36"/>
     </row>
     <row r="21" spans="1:8" s="6" customFormat="1" ht="4.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A21" s="23"/>
       <c r="B21" s="32"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="52"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="51"/>
     </row>
     <row r="22" spans="1:8" ht="57" customHeight="1" thickTop="1">
       <c r="A22" s="21"/>
-      <c r="B22" s="77" t="s">
+      <c r="B22" s="76" t="s">
         <v>14</v>
       </c>
       <c r="C22" s="18"/>
       <c r="D22" s="19"/>
       <c r="E22" s="19"/>
-      <c r="F22" s="48"/>
+      <c r="F22" s="47"/>
       <c r="G22" s="18"/>
-      <c r="H22" s="49"/>
+      <c r="H22" s="48"/>
     </row>
     <row r="23" spans="1:8" ht="54.75" customHeight="1">
       <c r="A23" s="21"/>
-      <c r="B23" s="78"/>
+      <c r="B23" s="77"/>
       <c r="C23" s="4"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
@@ -1829,7 +1952,7 @@
     </row>
     <row r="24" spans="1:8" ht="60" customHeight="1">
       <c r="A24" s="21"/>
-      <c r="B24" s="78"/>
+      <c r="B24" s="77"/>
       <c r="C24" s="4"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
@@ -1839,27 +1962,27 @@
     </row>
     <row r="25" spans="1:8" ht="51.75" customHeight="1" thickBot="1">
       <c r="A25" s="21"/>
-      <c r="B25" s="79"/>
+      <c r="B25" s="78"/>
       <c r="C25" s="33"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="41"/>
       <c r="F25" s="35"/>
       <c r="G25" s="33"/>
-      <c r="H25" s="43"/>
+      <c r="H25" s="42"/>
     </row>
     <row r="26" spans="1:8" ht="5.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A26" s="21"/>
       <c r="B26" s="38"/>
-      <c r="C26" s="65"/>
-      <c r="D26" s="66"/>
-      <c r="E26" s="44"/>
-      <c r="F26" s="45"/>
-      <c r="G26" s="46"/>
-      <c r="H26" s="47"/>
+      <c r="C26" s="64"/>
+      <c r="D26" s="65"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="45"/>
+      <c r="H26" s="46"/>
     </row>
     <row r="27" spans="1:8" ht="71.25" customHeight="1" thickTop="1">
       <c r="A27" s="21"/>
-      <c r="B27" s="70" t="s">
+      <c r="B27" s="69" t="s">
         <v>15</v>
       </c>
       <c r="C27" s="18"/>
@@ -1871,7 +1994,7 @@
     </row>
     <row r="28" spans="1:8" ht="63" customHeight="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="70"/>
+      <c r="B28" s="69"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="10"/>
@@ -1881,7 +2004,7 @@
     </row>
     <row r="29" spans="1:8" ht="62.25" customHeight="1">
       <c r="A29" s="21"/>
-      <c r="B29" s="70"/>
+      <c r="B29" s="69"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="3"/>
@@ -1891,7 +2014,7 @@
     </row>
     <row r="30" spans="1:8" ht="62.25" customHeight="1" thickBot="1">
       <c r="A30" s="21"/>
-      <c r="B30" s="70"/>
+      <c r="B30" s="69"/>
       <c r="C30" s="33"/>
       <c r="D30" s="33"/>
       <c r="E30" s="34"/>
@@ -1902,15 +2025,15 @@
     <row r="31" spans="1:8" ht="6.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A31" s="21"/>
       <c r="B31" s="37"/>
-      <c r="C31" s="64"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="67"/>
-      <c r="F31" s="67"/>
-      <c r="G31" s="68"/>
-      <c r="H31" s="46"/>
+      <c r="C31" s="63"/>
+      <c r="D31" s="44"/>
+      <c r="E31" s="66"/>
+      <c r="F31" s="66"/>
+      <c r="G31" s="67"/>
+      <c r="H31" s="45"/>
     </row>
     <row r="32" spans="1:8" ht="58.5" customHeight="1" thickTop="1">
-      <c r="B32" s="70" t="s">
+      <c r="B32" s="69" t="s">
         <v>16</v>
       </c>
       <c r="C32" s="18"/>
@@ -1921,7 +2044,7 @@
       <c r="H32" s="20"/>
     </row>
     <row r="33" spans="1:8" ht="48.75" customHeight="1">
-      <c r="B33" s="70"/>
+      <c r="B33" s="69"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="10"/>
@@ -1930,7 +2053,7 @@
       <c r="H33" s="13"/>
     </row>
     <row r="34" spans="1:8" ht="51.75" customHeight="1">
-      <c r="B34" s="70"/>
+      <c r="B34" s="69"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="3"/>
@@ -1940,7 +2063,7 @@
     </row>
     <row r="35" spans="1:8" ht="45.75" customHeight="1" thickBot="1">
       <c r="A35" s="21"/>
-      <c r="B35" s="80"/>
+      <c r="B35" s="79"/>
       <c r="C35" s="24"/>
       <c r="D35" s="24"/>
       <c r="E35" s="25"/>
@@ -1951,16 +2074,16 @@
     <row r="36" spans="1:8" ht="6.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A36" s="21"/>
       <c r="B36" s="37"/>
-      <c r="C36" s="46"/>
-      <c r="D36" s="44"/>
-      <c r="E36" s="45"/>
-      <c r="F36" s="53"/>
-      <c r="G36" s="46"/>
-      <c r="H36" s="47"/>
+      <c r="C36" s="45"/>
+      <c r="D36" s="43"/>
+      <c r="E36" s="44"/>
+      <c r="F36" s="52"/>
+      <c r="G36" s="45"/>
+      <c r="H36" s="46"/>
     </row>
     <row r="37" spans="1:8" ht="45" customHeight="1" thickTop="1">
       <c r="A37" s="21"/>
-      <c r="B37" s="69" t="s">
+      <c r="B37" s="68" t="s">
         <v>17</v>
       </c>
       <c r="C37" s="18"/>
@@ -1971,7 +2094,7 @@
       <c r="H37" s="20"/>
     </row>
     <row r="38" spans="1:8" ht="45.75" customHeight="1">
-      <c r="B38" s="70"/>
+      <c r="B38" s="69"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="10"/>
@@ -1980,7 +2103,7 @@
       <c r="H38" s="13"/>
     </row>
     <row r="39" spans="1:8" ht="45" customHeight="1">
-      <c r="B39" s="70"/>
+      <c r="B39" s="69"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
       <c r="E39" s="3"/>
@@ -1989,7 +2112,7 @@
       <c r="H39" s="13"/>
     </row>
     <row r="40" spans="1:8" ht="44.25" customHeight="1" thickBot="1">
-      <c r="B40" s="71"/>
+      <c r="B40" s="70"/>
       <c r="C40" s="24"/>
       <c r="D40" s="24"/>
       <c r="E40" s="25"/>
@@ -2041,7 +2164,7 @@
       <formula>$H22="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C17:H21 E22:E28 C22:D27 G22:G27">
+  <conditionalFormatting sqref="E22:E28 C22:D27 G22:G27 C17:H17 C19:H21 C18:E18 G18:H18">
     <cfRule type="expression" dxfId="19" priority="29" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
@@ -2141,7 +2264,7 @@
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="4">
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E34:E35 F35 E29:E30 E39:E40 F40">
       <formula1>"Organizational,Technical, Business ,Product"</formula1>
     </dataValidation>
@@ -2151,7 +2274,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G33:G35 G28:G30 G38:G40">
       <formula1>"1,2,3"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G17:G27 G31:G32 G36:G37">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G31:G32 G36:G37 G17:G27">
       <formula1>"High,Medium,Low"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Add review comments on data flow design
Add review comments on data flow design
</commit_message>
<xml_diff>
--- a/Design/Design document Peer Review sheet.xlsx
+++ b/Design/Design document Peer Review sheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\iti\project managment\design 2\Internet-Banking-System\Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\Internet-Banking-System\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="65">
   <si>
     <t>Priority</t>
   </si>
@@ -143,6 +143,104 @@
   <si>
     <t>missing to elaborate the response in case customer wants to  transfer amount of money greater than his balance to other bank or exceeds the amount he can transfer to a specific account 
  after (D)(3)</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_001</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q29
+BANK_SYS_SIQ_Q30</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-verifecation code is sent in case of register </t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q10
+BANK_SYS_SIQ_Q31
+BANK_SYS_SIQ_Q32</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
+  </si>
+  <si>
+    <t>1-when admin login or register sucessfully he will be redirected to admin home page not customer page
+2-verifecation code is sent in case of register not login
+3- to logi he need to enter user name ,password and national ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No SRS or CRS Related to this piece of design </t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_005</t>
+  </si>
+  <si>
+    <t>Admin will be redirectec to Admin Home Page not customer 
+home page</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q31</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_006</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the previous transaction page will not all the transactions directly .
+Transactions will be shown based  on which he will choosse from 
+the drop down menu 10,20,30 transactio </t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q22</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Missing</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Admin  can also add user not just remove </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Missing </t>
+  </si>
+  <si>
+    <t>What if the user wants to transfer money to account with the our
+ bank?</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q4
+BANK_SYS_SIQ_Q41</t>
+  </si>
+  <si>
+    <t>request to the user data base to ensure that befor transfere mony the user balance is begger than the transferred money</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q43</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the verification code is in case of registeration only </t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_002</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_003</t>
   </si>
 </sst>
 </file>
@@ -237,7 +335,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="45">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -807,6 +905,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color theme="8"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -814,7 +921,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -848,9 +955,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -920,9 +1024,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -956,18 +1057,12 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -1019,6 +1114,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1064,11 +1162,26 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1668,10 +1781,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A39" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1681,7 +1794,7 @@
     <col min="3" max="3" width="27.375" style="5" customWidth="1"/>
     <col min="4" max="4" width="36.75" style="5" customWidth="1"/>
     <col min="5" max="5" width="54.5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="27.875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="27.875" style="5" customWidth="1"/>
     <col min="7" max="7" width="18.125" style="2" customWidth="1"/>
     <col min="8" max="8" width="39.875" style="2" customWidth="1"/>
     <col min="9" max="16384" width="9" style="2"/>
@@ -1689,15 +1802,15 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15" thickBot="1"/>
     <row r="2" spans="1:8" ht="105" customHeight="1" thickBot="1">
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="73"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="70"/>
     </row>
     <row r="3" spans="1:8" ht="14.25" customHeight="1">
       <c r="C3" s="7"/>
@@ -1714,68 +1827,68 @@
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:8" ht="20.25" customHeight="1">
-      <c r="C5" s="80" t="s">
+      <c r="C5" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="80" t="s">
+      <c r="D5" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="80" t="s">
+      <c r="E5" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="80" t="s">
+      <c r="F5" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="80" t="s">
+      <c r="G5" s="77" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="23.25" customHeight="1" thickBot="1">
-      <c r="C6" s="81"/>
-      <c r="D6" s="81"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="81"/>
-      <c r="G6" s="81"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="78"/>
+      <c r="E6" s="79"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="78"/>
     </row>
     <row r="7" spans="1:8" ht="29.25" customHeight="1">
-      <c r="C7" s="12">
+      <c r="C7" s="11">
         <v>1</v>
       </c>
-      <c r="D7" s="62" t="s">
+      <c r="D7" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="61">
+      <c r="E7" s="57">
         <v>43713</v>
       </c>
-      <c r="F7" s="58"/>
+      <c r="F7" s="54"/>
       <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:8" ht="21.75" customHeight="1">
-      <c r="C8" s="53"/>
-      <c r="D8" s="54"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="59"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="55"/>
       <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:8" ht="21.75" customHeight="1">
-      <c r="C9" s="53"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="59"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="55"/>
       <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:8" ht="21.75" customHeight="1">
-      <c r="C10" s="53"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="59"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="55"/>
       <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:8" ht="20.25" customHeight="1">
-      <c r="C11" s="53"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="59"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="55"/>
       <c r="G11" s="9"/>
     </row>
     <row r="12" spans="1:8" ht="14.25" customHeight="1">
@@ -1802,65 +1915,65 @@
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:8" ht="14.25" customHeight="1" thickBot="1">
-      <c r="B15" s="15"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:8" ht="40.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A16" s="21"/>
-      <c r="B16" s="31" t="s">
+      <c r="A16" s="20"/>
+      <c r="B16" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="30" t="s">
+      <c r="D16" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="29" t="s">
+      <c r="E16" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="F16" s="28" t="s">
+      <c r="F16" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="G16" s="28" t="s">
+      <c r="G16" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="H16" s="27" t="s">
+      <c r="H16" s="26" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="139.5" customHeight="1" thickTop="1">
-      <c r="A17" s="21"/>
-      <c r="B17" s="74" t="s">
+      <c r="A17" s="20"/>
+      <c r="B17" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="40" t="s">
+      <c r="E17" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="19" t="s">
+      <c r="F17" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="G17" s="39" t="s">
+      <c r="G17" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="H17" s="83" t="s">
+      <c r="H17" s="64" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="57" customHeight="1" thickBot="1">
-      <c r="A18" s="21"/>
-      <c r="B18" s="69"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="66"/>
       <c r="C18" s="4" t="s">
         <v>21</v>
       </c>
@@ -1870,17 +1983,17 @@
       <c r="E18" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="84" t="s">
+      <c r="F18" s="86" t="s">
         <v>29</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H18" s="13"/>
+      <c r="H18" s="12"/>
     </row>
     <row r="19" spans="1:8" ht="54.75" customHeight="1">
-      <c r="A19" s="21"/>
-      <c r="B19" s="69"/>
+      <c r="A19" s="20"/>
+      <c r="B19" s="66"/>
       <c r="C19" s="4" t="s">
         <v>22</v>
       </c>
@@ -1896,262 +2009,516 @@
       <c r="G19" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H19" s="13"/>
+      <c r="H19" s="12"/>
     </row>
     <row r="20" spans="1:8" s="1" customFormat="1" ht="72.75" customHeight="1" thickBot="1">
-      <c r="A20" s="22"/>
-      <c r="B20" s="75"/>
-      <c r="C20" s="33" t="s">
+      <c r="A20" s="21"/>
+      <c r="B20" s="72"/>
+      <c r="C20" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="41" t="s">
+      <c r="D20" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="41" t="s">
+      <c r="E20" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="F20" s="35" t="s">
+      <c r="F20" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="33" t="s">
+      <c r="G20" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="H20" s="36"/>
+      <c r="H20" s="34"/>
     </row>
     <row r="21" spans="1:8" s="6" customFormat="1" ht="4.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A21" s="23"/>
-      <c r="B21" s="32"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="44"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="51"/>
+      <c r="A21" s="22"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="47"/>
     </row>
     <row r="22" spans="1:8" ht="57" customHeight="1" thickTop="1">
-      <c r="A22" s="21"/>
-      <c r="B22" s="76" t="s">
+      <c r="A22" s="20"/>
+      <c r="B22" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="47"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="48"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" s="18"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="45"/>
     </row>
     <row r="23" spans="1:8" ht="54.75" customHeight="1">
-      <c r="A23" s="21"/>
-      <c r="B23" s="77"/>
+      <c r="A23" s="20"/>
+      <c r="B23" s="74"/>
       <c r="C23" s="4"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
-      <c r="F23" s="11"/>
+      <c r="F23" s="10"/>
       <c r="G23" s="4"/>
-      <c r="H23" s="14"/>
+      <c r="H23" s="13"/>
     </row>
     <row r="24" spans="1:8" ht="60" customHeight="1">
-      <c r="A24" s="21"/>
-      <c r="B24" s="77"/>
+      <c r="A24" s="20"/>
+      <c r="B24" s="74"/>
       <c r="C24" s="4"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
-      <c r="F24" s="11"/>
+      <c r="F24" s="10"/>
       <c r="G24" s="4"/>
-      <c r="H24" s="14"/>
-    </row>
-    <row r="25" spans="1:8" ht="51.75" customHeight="1" thickBot="1">
-      <c r="A25" s="21"/>
-      <c r="B25" s="78"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="41"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="42"/>
-    </row>
-    <row r="26" spans="1:8" ht="5.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A26" s="21"/>
-      <c r="B26" s="38"/>
-      <c r="C26" s="64"/>
-      <c r="D26" s="65"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="44"/>
-      <c r="G26" s="45"/>
-      <c r="H26" s="46"/>
-    </row>
-    <row r="27" spans="1:8" ht="71.25" customHeight="1" thickTop="1">
-      <c r="A27" s="21"/>
-      <c r="B27" s="69" t="s">
+      <c r="H24" s="13"/>
+    </row>
+    <row r="25" spans="1:8" ht="60" customHeight="1">
+      <c r="A25" s="20"/>
+      <c r="B25" s="74"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="40"/>
+    </row>
+    <row r="26" spans="1:8" ht="60" customHeight="1">
+      <c r="A26" s="20"/>
+      <c r="B26" s="74"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="39"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="40"/>
+    </row>
+    <row r="27" spans="1:8" ht="60" customHeight="1">
+      <c r="A27" s="20"/>
+      <c r="B27" s="74"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="40"/>
+    </row>
+    <row r="28" spans="1:8" ht="60" customHeight="1">
+      <c r="A28" s="20"/>
+      <c r="B28" s="74"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="40"/>
+    </row>
+    <row r="29" spans="1:8" ht="51.75" customHeight="1" thickBot="1">
+      <c r="A29" s="20"/>
+      <c r="B29" s="75"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="40"/>
+    </row>
+    <row r="30" spans="1:8" ht="5.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A30" s="20"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="60"/>
+      <c r="D30" s="61"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="44"/>
+    </row>
+    <row r="31" spans="1:8" ht="71.25" customHeight="1" thickTop="1">
+      <c r="A31" s="20"/>
+      <c r="B31" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="20"/>
-    </row>
-    <row r="28" spans="1:8" ht="63" customHeight="1">
-      <c r="A28" s="21"/>
-      <c r="B28" s="69"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="13"/>
-    </row>
-    <row r="29" spans="1:8" ht="62.25" customHeight="1">
-      <c r="A29" s="21"/>
-      <c r="B29" s="69"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="13"/>
-    </row>
-    <row r="30" spans="1:8" ht="62.25" customHeight="1" thickBot="1">
-      <c r="A30" s="21"/>
-      <c r="B30" s="69"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="36"/>
-    </row>
-    <row r="31" spans="1:8" ht="6.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A31" s="21"/>
-      <c r="B31" s="37"/>
-      <c r="C31" s="63"/>
-      <c r="D31" s="44"/>
-      <c r="E31" s="66"/>
-      <c r="F31" s="66"/>
-      <c r="G31" s="67"/>
-      <c r="H31" s="45"/>
-    </row>
-    <row r="32" spans="1:8" ht="58.5" customHeight="1" thickTop="1">
-      <c r="B32" s="69" t="s">
+      <c r="C31" s="17"/>
+      <c r="D31" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="G31" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="H31" s="19"/>
+    </row>
+    <row r="32" spans="1:8" ht="63" customHeight="1">
+      <c r="A32" s="20"/>
+      <c r="B32" s="66"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H32" s="12"/>
+    </row>
+    <row r="33" spans="1:8" ht="62.25" customHeight="1">
+      <c r="A33" s="20"/>
+      <c r="B33" s="66"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H33" s="12"/>
+    </row>
+    <row r="34" spans="1:8" ht="62.25" customHeight="1">
+      <c r="A34" s="20"/>
+      <c r="B34" s="66"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="F34" s="39"/>
+      <c r="G34" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="H34" s="34"/>
+    </row>
+    <row r="35" spans="1:8" ht="62.25" customHeight="1">
+      <c r="A35" s="20"/>
+      <c r="B35" s="66"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="E35" s="85" t="s">
+        <v>47</v>
+      </c>
+      <c r="F35" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="G35" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="H35" s="34"/>
+    </row>
+    <row r="36" spans="1:8" ht="62.25" customHeight="1">
+      <c r="A36" s="20"/>
+      <c r="B36" s="66"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="E36" s="85" t="s">
+        <v>47</v>
+      </c>
+      <c r="F36" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="G36" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="H36" s="34"/>
+    </row>
+    <row r="37" spans="1:8" ht="62.25" customHeight="1">
+      <c r="A37" s="20"/>
+      <c r="B37" s="66"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="E37" s="85" t="s">
+        <v>51</v>
+      </c>
+      <c r="F37" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="G37" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="H37" s="34"/>
+    </row>
+    <row r="38" spans="1:8" ht="62.25" customHeight="1">
+      <c r="A38" s="20"/>
+      <c r="B38" s="66"/>
+      <c r="C38" s="32"/>
+      <c r="D38" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="E38" s="85" t="s">
+        <v>59</v>
+      </c>
+      <c r="F38" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="G38" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="H38" s="34"/>
+    </row>
+    <row r="39" spans="1:8" ht="62.25" customHeight="1">
+      <c r="A39" s="20"/>
+      <c r="B39" s="66"/>
+      <c r="C39" s="32"/>
+      <c r="D39" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="E39" s="85" t="s">
+        <v>57</v>
+      </c>
+      <c r="F39" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="G39" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="H39" s="34"/>
+    </row>
+    <row r="40" spans="1:8" ht="62.25" customHeight="1">
+      <c r="A40" s="20"/>
+      <c r="B40" s="66"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="E40" s="85" t="s">
+        <v>62</v>
+      </c>
+      <c r="F40" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="G40" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="H40" s="34"/>
+    </row>
+    <row r="41" spans="1:8" ht="62.25" customHeight="1">
+      <c r="A41" s="20"/>
+      <c r="B41" s="66"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="E41" s="85" t="s">
+        <v>62</v>
+      </c>
+      <c r="F41" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="G41" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="H41" s="34"/>
+    </row>
+    <row r="42" spans="1:8" ht="62.25" customHeight="1">
+      <c r="A42" s="20"/>
+      <c r="B42" s="66"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="E42" s="85" t="s">
+        <v>45</v>
+      </c>
+      <c r="F42" s="39"/>
+      <c r="G42" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="H42" s="34"/>
+    </row>
+    <row r="43" spans="1:8" ht="62.25" customHeight="1">
+      <c r="A43" s="20"/>
+      <c r="B43" s="66"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="32"/>
+      <c r="E43" s="85"/>
+      <c r="F43" s="39"/>
+      <c r="G43" s="32"/>
+      <c r="H43" s="34"/>
+    </row>
+    <row r="44" spans="1:8" ht="62.25" customHeight="1">
+      <c r="A44" s="20"/>
+      <c r="B44" s="66"/>
+      <c r="C44" s="32"/>
+      <c r="D44" s="32"/>
+      <c r="E44" s="85"/>
+      <c r="F44" s="39"/>
+      <c r="G44" s="32"/>
+      <c r="H44" s="34"/>
+    </row>
+    <row r="45" spans="1:8" ht="62.25" customHeight="1" thickBot="1">
+      <c r="A45" s="20"/>
+      <c r="B45" s="66"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="32"/>
+      <c r="E45" s="85"/>
+      <c r="F45" s="39"/>
+      <c r="G45" s="32"/>
+      <c r="H45" s="34"/>
+    </row>
+    <row r="46" spans="1:8" ht="6.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A46" s="20"/>
+      <c r="B46" s="35"/>
+      <c r="C46" s="59"/>
+      <c r="D46" s="42"/>
+      <c r="E46" s="62"/>
+      <c r="F46" s="62"/>
+      <c r="G46" s="63"/>
+      <c r="H46" s="43"/>
+    </row>
+    <row r="47" spans="1:8" ht="6.75" customHeight="1" thickTop="1">
+      <c r="A47" s="80"/>
+      <c r="B47" s="81"/>
+      <c r="C47" s="82"/>
+      <c r="D47" s="83"/>
+      <c r="E47" s="83"/>
+      <c r="F47" s="83"/>
+      <c r="G47" s="82"/>
+      <c r="H47" s="84"/>
+    </row>
+    <row r="48" spans="1:8" ht="58.5" customHeight="1">
+      <c r="B48" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="20"/>
-    </row>
-    <row r="33" spans="1:8" ht="48.75" customHeight="1">
-      <c r="B33" s="69"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="13"/>
-    </row>
-    <row r="34" spans="1:8" ht="51.75" customHeight="1">
-      <c r="B34" s="69"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="13"/>
-    </row>
-    <row r="35" spans="1:8" ht="45.75" customHeight="1" thickBot="1">
-      <c r="A35" s="21"/>
-      <c r="B35" s="79"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="24"/>
-      <c r="H35" s="26"/>
-    </row>
-    <row r="36" spans="1:8" ht="6.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A36" s="21"/>
-      <c r="B36" s="37"/>
-      <c r="C36" s="45"/>
-      <c r="D36" s="43"/>
-      <c r="E36" s="44"/>
-      <c r="F36" s="52"/>
-      <c r="G36" s="45"/>
-      <c r="H36" s="46"/>
-    </row>
-    <row r="37" spans="1:8" ht="45" customHeight="1" thickTop="1">
-      <c r="A37" s="21"/>
-      <c r="B37" s="68" t="s">
+      <c r="C48" s="17"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="17"/>
+      <c r="H48" s="19"/>
+    </row>
+    <row r="49" spans="1:8" ht="48.75" customHeight="1">
+      <c r="B49" s="66"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="12"/>
+    </row>
+    <row r="50" spans="1:8" ht="51.75" customHeight="1">
+      <c r="B50" s="66"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="12"/>
+    </row>
+    <row r="51" spans="1:8" ht="45.75" customHeight="1" thickBot="1">
+      <c r="A51" s="20"/>
+      <c r="B51" s="76"/>
+      <c r="C51" s="23"/>
+      <c r="D51" s="23"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="23"/>
+      <c r="G51" s="23"/>
+      <c r="H51" s="25"/>
+    </row>
+    <row r="52" spans="1:8" ht="6.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A52" s="20"/>
+      <c r="B52" s="35"/>
+      <c r="C52" s="43"/>
+      <c r="D52" s="41"/>
+      <c r="E52" s="42"/>
+      <c r="F52" s="48"/>
+      <c r="G52" s="43"/>
+      <c r="H52" s="44"/>
+    </row>
+    <row r="53" spans="1:8" ht="45" customHeight="1" thickTop="1">
+      <c r="A53" s="20"/>
+      <c r="B53" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="20"/>
-    </row>
-    <row r="38" spans="1:8" ht="45.75" customHeight="1">
-      <c r="B38" s="69"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="13"/>
-    </row>
-    <row r="39" spans="1:8" ht="45" customHeight="1">
-      <c r="B39" s="69"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="13"/>
-    </row>
-    <row r="40" spans="1:8" ht="44.25" customHeight="1" thickBot="1">
-      <c r="B40" s="70"/>
-      <c r="C40" s="24"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="24"/>
-      <c r="H40" s="26"/>
-    </row>
-    <row r="41" spans="1:8" ht="15" thickTop="1">
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-    </row>
-    <row r="42" spans="1:8">
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-    </row>
-    <row r="43" spans="1:8">
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-    </row>
-    <row r="44" spans="1:8">
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
+      <c r="C53" s="17"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="17"/>
+      <c r="H53" s="19"/>
+    </row>
+    <row r="54" spans="1:8" ht="45.75" customHeight="1">
+      <c r="B54" s="66"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="10"/>
+      <c r="F54" s="10"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="12"/>
+    </row>
+    <row r="55" spans="1:8" ht="45" customHeight="1">
+      <c r="B55" s="66"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="10"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="12"/>
+    </row>
+    <row r="56" spans="1:8" ht="44.25" customHeight="1" thickBot="1">
+      <c r="B56" s="67"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="23"/>
+      <c r="E56" s="24"/>
+      <c r="F56" s="23"/>
+      <c r="G56" s="23"/>
+      <c r="H56" s="25"/>
+    </row>
+    <row r="57" spans="1:8" ht="15" thickTop="1">
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B37:B40"/>
+    <mergeCell ref="B53:B56"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B17:B20"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="B22:B29"/>
+    <mergeCell ref="B48:B51"/>
+    <mergeCell ref="B31:B45"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="C5:C6"/>
@@ -2159,123 +2526,117 @@
     <mergeCell ref="E5:E6"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
-  <conditionalFormatting sqref="C29:E30 G28:H30 C28:D28 H22:H27">
+  <conditionalFormatting sqref="C33:E45 G32:H45 C32:D32 H22:H31">
     <cfRule type="expression" dxfId="20" priority="24" stopIfTrue="1">
       <formula>$H22="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E22:E28 C22:D27 G22:G27 C17:H17 C19:H21 C18:E18 G18:H18">
+  <conditionalFormatting sqref="E22:E32 C22:D31 G22:G31 C17:H17 C19:H21 C18:E18 G18:H18">
     <cfRule type="expression" dxfId="19" priority="29" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F22:F25 F28:F30">
+  <conditionalFormatting sqref="F22:F29 F32:F45">
     <cfRule type="expression" dxfId="18" priority="19" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F26">
+  <conditionalFormatting sqref="F30">
     <cfRule type="expression" dxfId="17" priority="18" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F27">
+  <conditionalFormatting sqref="F31">
     <cfRule type="expression" dxfId="16" priority="17" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C34:E35 G33:H35 C33:D33 H32">
+  <conditionalFormatting sqref="C50:E51 G49:H51 C49:D49 H48">
     <cfRule type="expression" dxfId="15" priority="15" stopIfTrue="1">
-      <formula>$H32="close"</formula>
+      <formula>$H48="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F35">
+  <conditionalFormatting sqref="F51">
     <cfRule type="expression" dxfId="14" priority="14" stopIfTrue="1">
-      <formula>$H35="close"</formula>
+      <formula>$H51="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E32:E33 C32:D32 G32">
+  <conditionalFormatting sqref="E48:E49 C48:D48 G48">
     <cfRule type="expression" dxfId="13" priority="16" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F33:F34">
+  <conditionalFormatting sqref="F49:F50">
     <cfRule type="expression" dxfId="12" priority="13" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F32">
+  <conditionalFormatting sqref="F48">
     <cfRule type="expression" dxfId="11" priority="12" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H31">
+  <conditionalFormatting sqref="H46:H47">
     <cfRule type="expression" dxfId="10" priority="10" stopIfTrue="1">
-      <formula>$H31="close"</formula>
+      <formula>$H46="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C31:E31 G31">
+  <conditionalFormatting sqref="C46:E47 G46:G47">
     <cfRule type="expression" dxfId="9" priority="11" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F31">
+  <conditionalFormatting sqref="F46:F47">
     <cfRule type="expression" dxfId="8" priority="9" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H36">
+  <conditionalFormatting sqref="H52">
     <cfRule type="expression" dxfId="7" priority="7" stopIfTrue="1">
-      <formula>$H36="close"</formula>
+      <formula>$H52="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C36:E36 G36">
+  <conditionalFormatting sqref="C52:E52 G52">
     <cfRule type="expression" dxfId="6" priority="8" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F36">
+  <conditionalFormatting sqref="F52">
     <cfRule type="expression" dxfId="5" priority="6" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C39:E40 G38:H40 C38:D38 H37">
+  <conditionalFormatting sqref="C55:E56 G54:H56 C54:D54 H53">
     <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
-      <formula>$H37="close"</formula>
+      <formula>$H53="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F40">
+  <conditionalFormatting sqref="F56">
     <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
-      <formula>$H40="close"</formula>
+      <formula>$H56="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E37:E38 C37:D37 G37">
+  <conditionalFormatting sqref="E53:E54 C53:D53 G53">
     <cfRule type="expression" dxfId="2" priority="5" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F38:F39">
+  <conditionalFormatting sqref="F54:F55">
     <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F37">
+  <conditionalFormatting sqref="F53">
     <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E34:E35 F35 E29:E30 E39:E40 F40">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F56 F51">
       <formula1>"Organizational,Technical, Business ,Product"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H22:H40">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H22:H56">
       <formula1>"close,open"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G33:G35 G28:G30 G38:G40">
-      <formula1>"1,2,3"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G31:G32 G36:G37 G17:G27">
-      <formula1>"High,Medium,Low"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51200000000000001" footer="0.51200000000000001"/>

</xml_diff>

<commit_message>
Update Design document Peer Review sheet.xlsx
Update design document peer review sheet
</commit_message>
<xml_diff>
--- a/Design/Design document Peer Review sheet.xlsx
+++ b/Design/Design document Peer Review sheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\Internet-Banking-System\Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed\Documents\GitHub\Internet-Banking-System\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2700" windowWidth="20490" windowHeight="7890"/>
+    <workbookView xWindow="0" yWindow="3150" windowWidth="20490" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="SRS-PR Sheet" sheetId="1" r:id="rId1"/>
@@ -27,12 +27,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="72">
   <si>
     <t>Priority</t>
-  </si>
-  <si>
-    <t>Reviewed by</t>
   </si>
   <si>
     <t>Comments</t>
@@ -242,12 +239,36 @@
   <si>
     <t>Bank_Sys_DM_CST_003</t>
   </si>
+  <si>
+    <t>Review by</t>
+  </si>
+  <si>
+    <t>Khadija</t>
+  </si>
+  <si>
+    <t>Hassan</t>
+  </si>
+  <si>
+    <t>Sondos</t>
+  </si>
+  <si>
+    <t>Salsabeel</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Comment</t>
+  </si>
+  <si>
+    <t>Initiate design document peer review</t>
+  </si>
+  <si>
+    <t>Update peer review sheet</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -320,8 +341,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -334,8 +361,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="46">
+  <borders count="47">
     <border>
       <left/>
       <right/>
@@ -365,34 +398,6 @@
       <right style="thin">
         <color theme="1"/>
       </right>
-      <top style="medium">
-        <color rgb="FF5B9BD5"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
       <top style="thin">
         <color theme="1"/>
       </top>
@@ -419,17 +424,6 @@
       <right style="thin">
         <color theme="1"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
       <top style="medium">
         <color rgb="FF5B9BD5"/>
       </top>
@@ -463,21 +457,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color theme="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -487,19 +466,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color theme="8"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thick">
         <color theme="8"/>
@@ -523,21 +489,6 @@
       </left>
       <right style="thin">
         <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thick">
-        <color theme="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color theme="8"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
@@ -650,34 +601,49 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color theme="8"/>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="8"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color theme="8"/>
+      </top>
+      <bottom style="thick">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color theme="8"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color theme="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thick">
         <color theme="8"/>
       </left>
-      <right/>
+      <right style="thick">
+        <color theme="8"/>
+      </right>
       <top style="thick">
         <color theme="8"/>
       </top>
@@ -687,39 +653,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color theme="8"/>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color theme="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color theme="8"/>
-      </left>
-      <right style="thick">
-        <color theme="8"/>
-      </right>
-      <top style="thick">
-        <color theme="8"/>
-      </top>
-      <bottom style="thick">
-        <color theme="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color theme="8"/>
       </right>
       <top style="thick">
         <color theme="8"/>
@@ -733,38 +671,12 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
-        <color theme="8"/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
         <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -800,19 +712,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF5B9BD5"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thick">
         <color theme="8"/>
       </left>
@@ -911,6 +810,135 @@
       </left>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="8"/>
+      </right>
+      <top style="thick">
+        <color theme="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="8"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color theme="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color theme="8"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -921,7 +949,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -946,241 +974,307 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="43" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1781,10 +1875,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A39" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1796,723 +1890,849 @@
     <col min="5" max="5" width="54.5" style="2" customWidth="1"/>
     <col min="6" max="6" width="27.875" style="5" customWidth="1"/>
     <col min="7" max="7" width="18.125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="39.875" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="2"/>
+    <col min="8" max="10" width="39.875" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1"/>
-    <row r="2" spans="1:8" ht="105" customHeight="1" thickBot="1">
-      <c r="B2" s="68" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="70"/>
-    </row>
-    <row r="3" spans="1:8" ht="14.25" customHeight="1">
+    <row r="1" spans="1:10" ht="15" thickBot="1"/>
+    <row r="2" spans="1:10" ht="105" customHeight="1" thickBot="1">
+      <c r="B2" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+    </row>
+    <row r="3" spans="1:10" ht="14.25" customHeight="1">
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="1:8" ht="14.25" customHeight="1">
+    <row r="4" spans="1:10" ht="14.25" customHeight="1">
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
     </row>
-    <row r="5" spans="1:8" ht="20.25" customHeight="1">
-      <c r="C5" s="77" t="s">
+    <row r="5" spans="1:10" ht="20.25" customHeight="1">
+      <c r="C5" s="69" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="77" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="77" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="77" t="s">
+      <c r="E5" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="105" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" s="100"/>
+    </row>
+    <row r="6" spans="1:10" ht="23.25" customHeight="1" thickBot="1">
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="104"/>
+      <c r="G6" s="100"/>
+    </row>
+    <row r="7" spans="1:10" ht="29.25" customHeight="1">
+      <c r="C7" s="9">
         <v>1</v>
       </c>
-      <c r="G5" s="77" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="23.25" customHeight="1" thickBot="1">
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="79"/>
-      <c r="F6" s="78"/>
-      <c r="G6" s="78"/>
-    </row>
-    <row r="7" spans="1:8" ht="29.25" customHeight="1">
-      <c r="C7" s="11">
-        <v>1</v>
-      </c>
-      <c r="D7" s="58" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="57">
+      <c r="D7" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="71">
         <v>43713</v>
       </c>
-      <c r="F7" s="54"/>
-      <c r="G7" s="8"/>
-    </row>
-    <row r="8" spans="1:8" ht="21.75" customHeight="1">
-      <c r="C8" s="49"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="55"/>
-      <c r="G8" s="9"/>
-    </row>
-    <row r="9" spans="1:8" ht="21.75" customHeight="1">
-      <c r="C9" s="49"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="56"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="9"/>
-    </row>
-    <row r="10" spans="1:8" ht="21.75" customHeight="1">
-      <c r="C10" s="49"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="9"/>
-    </row>
-    <row r="11" spans="1:8" ht="20.25" customHeight="1">
-      <c r="C11" s="49"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="9"/>
-    </row>
-    <row r="12" spans="1:8" ht="14.25" customHeight="1">
+      <c r="F7" s="108" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" s="100"/>
+    </row>
+    <row r="8" spans="1:10" ht="21.75" customHeight="1">
+      <c r="C8" s="106">
+        <v>2</v>
+      </c>
+      <c r="D8" s="107" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="71">
+        <v>43743</v>
+      </c>
+      <c r="F8" s="108" t="s">
+        <v>71</v>
+      </c>
+      <c r="G8" s="100"/>
+    </row>
+    <row r="9" spans="1:10" ht="21.75" customHeight="1">
+      <c r="C9" s="40"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="102"/>
+      <c r="G9" s="100"/>
+    </row>
+    <row r="10" spans="1:10" ht="21.75" customHeight="1">
+      <c r="C10" s="40"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="72"/>
+      <c r="F10" s="101"/>
+      <c r="G10" s="100"/>
+    </row>
+    <row r="11" spans="1:10" ht="20.25" customHeight="1">
+      <c r="C11" s="40"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="72"/>
+      <c r="F11" s="102"/>
+      <c r="G11" s="100"/>
+    </row>
+    <row r="12" spans="1:10" ht="14.25" customHeight="1">
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
+      <c r="F12" s="103"/>
+      <c r="G12" s="100"/>
       <c r="H12" s="7"/>
-    </row>
-    <row r="13" spans="1:8" ht="14.25" customHeight="1">
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" ht="14.25" customHeight="1">
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
+      <c r="F13" s="100"/>
+      <c r="G13" s="100"/>
       <c r="H13" s="7"/>
-    </row>
-    <row r="14" spans="1:8" ht="14.25" customHeight="1">
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" ht="14.25" customHeight="1">
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:8" ht="14.25" customHeight="1" thickBot="1">
-      <c r="B15" s="14"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-    </row>
-    <row r="16" spans="1:8" ht="40.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A16" s="20"/>
-      <c r="B16" s="30" t="s">
+    <row r="15" spans="1:10" ht="14.25" customHeight="1" thickBot="1">
+      <c r="B15" s="10"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="75"/>
+      <c r="J15" s="75"/>
+    </row>
+    <row r="16" spans="1:10" ht="40.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A16" s="15"/>
+      <c r="B16" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="I16" s="76" t="s">
+        <v>64</v>
+      </c>
+      <c r="J16" s="84" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="139.5" customHeight="1" thickTop="1">
+      <c r="A17" s="15"/>
+      <c r="B17" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="G16" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="H16" s="26" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="139.5" customHeight="1" thickTop="1">
-      <c r="A17" s="20"/>
-      <c r="B17" s="71" t="s">
+      <c r="C17" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="I17" s="78" t="s">
+        <v>65</v>
+      </c>
+      <c r="J17" s="97">
+        <v>43743</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="57" customHeight="1" thickBot="1">
+      <c r="A18" s="15"/>
+      <c r="B18" s="58"/>
+      <c r="C18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="56" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" s="3"/>
+      <c r="I18" s="78"/>
+      <c r="J18" s="96"/>
+    </row>
+    <row r="19" spans="1:10" ht="54.75" customHeight="1">
+      <c r="A19" s="15"/>
+      <c r="B19" s="58"/>
+      <c r="C19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" s="3"/>
+      <c r="I19" s="78"/>
+      <c r="J19" s="96"/>
+    </row>
+    <row r="20" spans="1:10" s="1" customFormat="1" ht="72.75" customHeight="1" thickBot="1">
+      <c r="A20" s="16"/>
+      <c r="B20" s="64"/>
+      <c r="C20" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20" s="19"/>
+      <c r="I20" s="78"/>
+      <c r="J20" s="96"/>
+    </row>
+    <row r="21" spans="1:10" s="6" customFormat="1" ht="4.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A21" s="17"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="77"/>
+      <c r="J21" s="83"/>
+    </row>
+    <row r="22" spans="1:10" ht="57" customHeight="1" thickTop="1">
+      <c r="A22" s="15"/>
+      <c r="B22" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="G17" s="37" t="s">
-        <v>24</v>
-      </c>
-      <c r="H17" s="64" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="57" customHeight="1" thickBot="1">
-      <c r="A18" s="20"/>
-      <c r="B18" s="66"/>
-      <c r="C18" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="F18" s="86" t="s">
-        <v>29</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H18" s="12"/>
-    </row>
-    <row r="19" spans="1:8" ht="54.75" customHeight="1">
-      <c r="A19" s="20"/>
-      <c r="B19" s="66"/>
-      <c r="C19" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H19" s="12"/>
-    </row>
-    <row r="20" spans="1:8" s="1" customFormat="1" ht="72.75" customHeight="1" thickBot="1">
-      <c r="A20" s="21"/>
-      <c r="B20" s="72"/>
-      <c r="C20" s="32" t="s">
+      <c r="C22" s="13"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" s="14"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="79" t="s">
+        <v>66</v>
+      </c>
+      <c r="J22" s="98"/>
+    </row>
+    <row r="23" spans="1:10" ht="54.75" customHeight="1">
+      <c r="A23" s="15"/>
+      <c r="B23" s="66"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="79"/>
+      <c r="J23" s="95"/>
+    </row>
+    <row r="24" spans="1:10" ht="60" customHeight="1">
+      <c r="A24" s="15"/>
+      <c r="B24" s="66"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="79"/>
+      <c r="J24" s="95"/>
+    </row>
+    <row r="25" spans="1:10" ht="60" customHeight="1">
+      <c r="A25" s="15"/>
+      <c r="B25" s="66"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="79"/>
+      <c r="J25" s="95"/>
+    </row>
+    <row r="26" spans="1:10" ht="60" customHeight="1">
+      <c r="A26" s="15"/>
+      <c r="B26" s="66"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="79"/>
+      <c r="J26" s="95"/>
+    </row>
+    <row r="27" spans="1:10" ht="60" customHeight="1">
+      <c r="A27" s="15"/>
+      <c r="B27" s="66"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="79"/>
+      <c r="J27" s="95"/>
+    </row>
+    <row r="28" spans="1:10" ht="60" customHeight="1">
+      <c r="A28" s="15"/>
+      <c r="B28" s="66"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="79"/>
+      <c r="J28" s="95"/>
+    </row>
+    <row r="29" spans="1:10" ht="51.75" customHeight="1" thickBot="1">
+      <c r="A29" s="15"/>
+      <c r="B29" s="67"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="79"/>
+      <c r="J29" s="95"/>
+    </row>
+    <row r="30" spans="1:10" ht="5.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A30" s="15"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="35"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="52"/>
+      <c r="J30" s="54"/>
+    </row>
+    <row r="31" spans="1:10" ht="71.25" customHeight="1" thickTop="1">
+      <c r="A31" s="15"/>
+      <c r="B31" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="13"/>
+      <c r="D31" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="G31" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="E20" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="F20" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="G20" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="H20" s="34"/>
-    </row>
-    <row r="21" spans="1:8" s="6" customFormat="1" ht="4.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A21" s="22"/>
-      <c r="B21" s="31"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="47"/>
-    </row>
-    <row r="22" spans="1:8" ht="57" customHeight="1" thickTop="1">
-      <c r="A22" s="20"/>
-      <c r="B22" s="73" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="F22" s="18"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="45"/>
-    </row>
-    <row r="23" spans="1:8" ht="54.75" customHeight="1">
-      <c r="A23" s="20"/>
-      <c r="B23" s="74"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="13"/>
-    </row>
-    <row r="24" spans="1:8" ht="60" customHeight="1">
-      <c r="A24" s="20"/>
-      <c r="B24" s="74"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="13"/>
-    </row>
-    <row r="25" spans="1:8" ht="60" customHeight="1">
-      <c r="A25" s="20"/>
-      <c r="B25" s="74"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="32"/>
-      <c r="H25" s="40"/>
-    </row>
-    <row r="26" spans="1:8" ht="60" customHeight="1">
-      <c r="A26" s="20"/>
-      <c r="B26" s="74"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="40"/>
-    </row>
-    <row r="27" spans="1:8" ht="60" customHeight="1">
-      <c r="A27" s="20"/>
-      <c r="B27" s="74"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="39"/>
-      <c r="G27" s="32"/>
-      <c r="H27" s="40"/>
-    </row>
-    <row r="28" spans="1:8" ht="60" customHeight="1">
-      <c r="A28" s="20"/>
-      <c r="B28" s="74"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="40"/>
-    </row>
-    <row r="29" spans="1:8" ht="51.75" customHeight="1" thickBot="1">
-      <c r="A29" s="20"/>
-      <c r="B29" s="75"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="40"/>
-    </row>
-    <row r="30" spans="1:8" ht="5.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A30" s="20"/>
-      <c r="B30" s="36"/>
-      <c r="C30" s="60"/>
-      <c r="D30" s="61"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="44"/>
-    </row>
-    <row r="31" spans="1:8" ht="71.25" customHeight="1" thickTop="1">
-      <c r="A31" s="20"/>
-      <c r="B31" s="66" t="s">
-        <v>15</v>
-      </c>
-      <c r="C31" s="17"/>
-      <c r="D31" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="E31" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="F31" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="G31" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="H31" s="19"/>
-    </row>
-    <row r="32" spans="1:8" ht="63" customHeight="1">
-      <c r="A32" s="20"/>
-      <c r="B32" s="66"/>
+      <c r="H31" s="86"/>
+      <c r="I31" s="79" t="s">
+        <v>67</v>
+      </c>
+      <c r="J31" s="98">
+        <v>43743</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="63" customHeight="1">
+      <c r="A32" s="15"/>
+      <c r="B32" s="58"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E32" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E32" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="F32" s="10" t="s">
-        <v>37</v>
+      <c r="F32" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H32" s="12"/>
-    </row>
-    <row r="33" spans="1:8" ht="62.25" customHeight="1">
-      <c r="A33" s="20"/>
-      <c r="B33" s="66"/>
+        <v>40</v>
+      </c>
+      <c r="H32" s="3"/>
+      <c r="I32" s="79"/>
+      <c r="J32" s="95"/>
+    </row>
+    <row r="33" spans="1:10" ht="62.25" customHeight="1">
+      <c r="A33" s="15"/>
+      <c r="B33" s="58"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E33" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="F33" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H33" s="3"/>
+      <c r="I33" s="79"/>
+      <c r="J33" s="95"/>
+    </row>
+    <row r="34" spans="1:10" ht="62.25" customHeight="1">
+      <c r="A34" s="15"/>
+      <c r="B34" s="58"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E34" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="F34" s="32"/>
+      <c r="G34" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="H34" s="27"/>
+      <c r="I34" s="79"/>
+      <c r="J34" s="95"/>
+    </row>
+    <row r="35" spans="1:10" ht="62.25" customHeight="1">
+      <c r="A35" s="15"/>
+      <c r="B35" s="58"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="E35" s="55" t="s">
+        <v>46</v>
+      </c>
+      <c r="F35" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="G35" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="H35" s="27"/>
+      <c r="I35" s="79"/>
+      <c r="J35" s="95"/>
+    </row>
+    <row r="36" spans="1:10" ht="62.25" customHeight="1">
+      <c r="A36" s="15"/>
+      <c r="B36" s="58"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="E36" s="55" t="s">
+        <v>46</v>
+      </c>
+      <c r="F36" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="G36" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="H36" s="27"/>
+      <c r="I36" s="79"/>
+      <c r="J36" s="95"/>
+    </row>
+    <row r="37" spans="1:10" ht="62.25" customHeight="1">
+      <c r="A37" s="15"/>
+      <c r="B37" s="58"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="E37" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="F37" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="G37" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="H37" s="27"/>
+      <c r="I37" s="79"/>
+      <c r="J37" s="95"/>
+    </row>
+    <row r="38" spans="1:10" ht="62.25" customHeight="1">
+      <c r="A38" s="15"/>
+      <c r="B38" s="58"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="F33" s="10" t="s">
+      <c r="E38" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="F38" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="G38" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="H38" s="27"/>
+      <c r="I38" s="79"/>
+      <c r="J38" s="95"/>
+    </row>
+    <row r="39" spans="1:10" ht="62.25" customHeight="1">
+      <c r="A39" s="15"/>
+      <c r="B39" s="58"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="E39" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="F39" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="G39" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="H39" s="27"/>
+      <c r="I39" s="79"/>
+      <c r="J39" s="95"/>
+    </row>
+    <row r="40" spans="1:10" ht="62.25" customHeight="1">
+      <c r="A40" s="15"/>
+      <c r="B40" s="58"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="E40" s="55" t="s">
+        <v>61</v>
+      </c>
+      <c r="F40" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="G40" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="H40" s="27"/>
+      <c r="I40" s="79"/>
+      <c r="J40" s="95"/>
+    </row>
+    <row r="41" spans="1:10" ht="62.25" customHeight="1">
+      <c r="A41" s="15"/>
+      <c r="B41" s="58"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="E41" s="55" t="s">
+        <v>61</v>
+      </c>
+      <c r="F41" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="G41" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="G33" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H33" s="12"/>
-    </row>
-    <row r="34" spans="1:8" ht="62.25" customHeight="1">
-      <c r="A34" s="20"/>
-      <c r="B34" s="66"/>
-      <c r="C34" s="32"/>
-      <c r="D34" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="E34" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="F34" s="39"/>
-      <c r="G34" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="H34" s="34"/>
-    </row>
-    <row r="35" spans="1:8" ht="62.25" customHeight="1">
-      <c r="A35" s="20"/>
-      <c r="B35" s="66"/>
-      <c r="C35" s="32"/>
-      <c r="D35" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="E35" s="85" t="s">
-        <v>47</v>
-      </c>
-      <c r="F35" s="39" t="s">
-        <v>48</v>
-      </c>
-      <c r="G35" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="H35" s="34"/>
-    </row>
-    <row r="36" spans="1:8" ht="62.25" customHeight="1">
-      <c r="A36" s="20"/>
-      <c r="B36" s="66"/>
-      <c r="C36" s="32"/>
-      <c r="D36" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="E36" s="85" t="s">
-        <v>47</v>
-      </c>
-      <c r="F36" s="39" t="s">
-        <v>48</v>
-      </c>
-      <c r="G36" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="H36" s="34"/>
-    </row>
-    <row r="37" spans="1:8" ht="62.25" customHeight="1">
-      <c r="A37" s="20"/>
-      <c r="B37" s="66"/>
-      <c r="C37" s="32"/>
-      <c r="D37" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="E37" s="85" t="s">
-        <v>51</v>
-      </c>
-      <c r="F37" s="39" t="s">
-        <v>52</v>
-      </c>
-      <c r="G37" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="H37" s="34"/>
-    </row>
-    <row r="38" spans="1:8" ht="62.25" customHeight="1">
-      <c r="A38" s="20"/>
-      <c r="B38" s="66"/>
-      <c r="C38" s="32"/>
-      <c r="D38" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="E38" s="85" t="s">
-        <v>59</v>
-      </c>
-      <c r="F38" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="G38" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="H38" s="34"/>
-    </row>
-    <row r="39" spans="1:8" ht="62.25" customHeight="1">
-      <c r="A39" s="20"/>
-      <c r="B39" s="66"/>
-      <c r="C39" s="32"/>
-      <c r="D39" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="E39" s="85" t="s">
-        <v>57</v>
-      </c>
-      <c r="F39" s="39" t="s">
-        <v>58</v>
-      </c>
-      <c r="G39" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="H39" s="34"/>
-    </row>
-    <row r="40" spans="1:8" ht="62.25" customHeight="1">
-      <c r="A40" s="20"/>
-      <c r="B40" s="66"/>
-      <c r="C40" s="32"/>
-      <c r="D40" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="E40" s="85" t="s">
-        <v>62</v>
-      </c>
-      <c r="F40" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="G40" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="H40" s="34"/>
-    </row>
-    <row r="41" spans="1:8" ht="62.25" customHeight="1">
-      <c r="A41" s="20"/>
-      <c r="B41" s="66"/>
-      <c r="C41" s="32"/>
-      <c r="D41" s="32" t="s">
+      <c r="H41" s="27"/>
+      <c r="I41" s="79"/>
+      <c r="J41" s="95"/>
+    </row>
+    <row r="42" spans="1:10" ht="62.25" customHeight="1">
+      <c r="A42" s="15"/>
+      <c r="B42" s="58"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="E41" s="85" t="s">
-        <v>62</v>
-      </c>
-      <c r="F41" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="G41" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="H41" s="34"/>
-    </row>
-    <row r="42" spans="1:8" ht="62.25" customHeight="1">
-      <c r="A42" s="20"/>
-      <c r="B42" s="66"/>
-      <c r="C42" s="32"/>
-      <c r="D42" s="32" t="s">
-        <v>64</v>
-      </c>
-      <c r="E42" s="85" t="s">
-        <v>45</v>
-      </c>
-      <c r="F42" s="39"/>
-      <c r="G42" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="H42" s="34"/>
-    </row>
-    <row r="43" spans="1:8" ht="62.25" customHeight="1">
-      <c r="A43" s="20"/>
-      <c r="B43" s="66"/>
-      <c r="C43" s="32"/>
-      <c r="D43" s="32"/>
-      <c r="E43" s="85"/>
-      <c r="F43" s="39"/>
-      <c r="G43" s="32"/>
-      <c r="H43" s="34"/>
-    </row>
-    <row r="44" spans="1:8" ht="62.25" customHeight="1">
-      <c r="A44" s="20"/>
-      <c r="B44" s="66"/>
-      <c r="C44" s="32"/>
-      <c r="D44" s="32"/>
-      <c r="E44" s="85"/>
-      <c r="F44" s="39"/>
-      <c r="G44" s="32"/>
-      <c r="H44" s="34"/>
-    </row>
-    <row r="45" spans="1:8" ht="62.25" customHeight="1" thickBot="1">
-      <c r="A45" s="20"/>
-      <c r="B45" s="66"/>
-      <c r="C45" s="32"/>
-      <c r="D45" s="32"/>
-      <c r="E45" s="85"/>
-      <c r="F45" s="39"/>
-      <c r="G45" s="32"/>
-      <c r="H45" s="34"/>
-    </row>
-    <row r="46" spans="1:8" ht="6.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A46" s="20"/>
-      <c r="B46" s="35"/>
-      <c r="C46" s="59"/>
-      <c r="D46" s="42"/>
-      <c r="E46" s="62"/>
-      <c r="F46" s="62"/>
-      <c r="G46" s="63"/>
-      <c r="H46" s="43"/>
-    </row>
-    <row r="47" spans="1:8" ht="6.75" customHeight="1" thickTop="1">
-      <c r="A47" s="80"/>
-      <c r="B47" s="81"/>
-      <c r="C47" s="82"/>
-      <c r="D47" s="83"/>
-      <c r="E47" s="83"/>
-      <c r="F47" s="83"/>
-      <c r="G47" s="82"/>
-      <c r="H47" s="84"/>
-    </row>
-    <row r="48" spans="1:8" ht="58.5" customHeight="1">
-      <c r="B48" s="66" t="s">
-        <v>16</v>
-      </c>
-      <c r="C48" s="17"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="17"/>
-      <c r="H48" s="19"/>
-    </row>
-    <row r="49" spans="1:8" ht="48.75" customHeight="1">
-      <c r="B49" s="66"/>
+      <c r="E42" s="55" t="s">
+        <v>44</v>
+      </c>
+      <c r="F42" s="32"/>
+      <c r="G42" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="H42" s="27"/>
+      <c r="I42" s="79"/>
+      <c r="J42" s="95"/>
+    </row>
+    <row r="43" spans="1:10" ht="62.25" customHeight="1">
+      <c r="A43" s="15"/>
+      <c r="B43" s="58"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="55"/>
+      <c r="F43" s="32"/>
+      <c r="G43" s="26"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="79"/>
+      <c r="J43" s="95"/>
+    </row>
+    <row r="44" spans="1:10" ht="62.25" customHeight="1">
+      <c r="A44" s="15"/>
+      <c r="B44" s="58"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="55"/>
+      <c r="F44" s="32"/>
+      <c r="G44" s="26"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="79"/>
+      <c r="J44" s="95"/>
+    </row>
+    <row r="45" spans="1:10" ht="62.25" customHeight="1" thickBot="1">
+      <c r="A45" s="15"/>
+      <c r="B45" s="58"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="55"/>
+      <c r="F45" s="32"/>
+      <c r="G45" s="26"/>
+      <c r="H45" s="19"/>
+      <c r="I45" s="79"/>
+      <c r="J45" s="95"/>
+    </row>
+    <row r="46" spans="1:10" ht="6.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A46" s="15"/>
+      <c r="B46" s="28"/>
+      <c r="C46" s="45"/>
+      <c r="D46" s="34"/>
+      <c r="E46" s="48"/>
+      <c r="F46" s="48"/>
+      <c r="G46" s="49"/>
+      <c r="H46" s="35"/>
+      <c r="I46" s="52"/>
+      <c r="J46" s="54"/>
+    </row>
+    <row r="47" spans="1:10" ht="6.75" customHeight="1" thickTop="1">
+      <c r="A47" s="50"/>
+      <c r="B47" s="51"/>
+      <c r="C47" s="52"/>
+      <c r="D47" s="53"/>
+      <c r="E47" s="53"/>
+      <c r="F47" s="53"/>
+      <c r="G47" s="52"/>
+      <c r="H47" s="54"/>
+      <c r="I47" s="52"/>
+      <c r="J47" s="54"/>
+    </row>
+    <row r="48" spans="1:10" ht="58.5" customHeight="1">
+      <c r="B48" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="C48" s="13"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="87"/>
+      <c r="I48" s="90" t="s">
+        <v>67</v>
+      </c>
+      <c r="J48" s="81"/>
+    </row>
+    <row r="49" spans="1:10" ht="48.75" customHeight="1">
+      <c r="B49" s="58"/>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
-      <c r="E49" s="10"/>
-      <c r="F49" s="10"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
       <c r="G49" s="4"/>
-      <c r="H49" s="12"/>
-    </row>
-    <row r="50" spans="1:8" ht="51.75" customHeight="1">
-      <c r="B50" s="66"/>
+      <c r="H49" s="88"/>
+      <c r="I49" s="91"/>
+      <c r="J49" s="81"/>
+    </row>
+    <row r="50" spans="1:10" ht="51.75" customHeight="1">
+      <c r="B50" s="58"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
       <c r="E50" s="3"/>
-      <c r="F50" s="10"/>
+      <c r="F50" s="8"/>
       <c r="G50" s="4"/>
-      <c r="H50" s="12"/>
-    </row>
-    <row r="51" spans="1:8" ht="45.75" customHeight="1" thickBot="1">
-      <c r="A51" s="20"/>
-      <c r="B51" s="76"/>
-      <c r="C51" s="23"/>
-      <c r="D51" s="23"/>
-      <c r="E51" s="24"/>
-      <c r="F51" s="23"/>
-      <c r="G51" s="23"/>
-      <c r="H51" s="25"/>
-    </row>
-    <row r="52" spans="1:8" ht="6.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A52" s="20"/>
-      <c r="B52" s="35"/>
-      <c r="C52" s="43"/>
-      <c r="D52" s="41"/>
-      <c r="E52" s="42"/>
-      <c r="F52" s="48"/>
-      <c r="G52" s="43"/>
-      <c r="H52" s="44"/>
-    </row>
-    <row r="53" spans="1:8" ht="45" customHeight="1" thickTop="1">
-      <c r="A53" s="20"/>
-      <c r="B53" s="65" t="s">
-        <v>17</v>
-      </c>
-      <c r="C53" s="17"/>
-      <c r="D53" s="18"/>
-      <c r="E53" s="18"/>
-      <c r="F53" s="18"/>
-      <c r="G53" s="17"/>
-      <c r="H53" s="19"/>
-    </row>
-    <row r="54" spans="1:8" ht="45.75" customHeight="1">
-      <c r="B54" s="66"/>
+      <c r="H50" s="88"/>
+      <c r="I50" s="91"/>
+      <c r="J50" s="81"/>
+    </row>
+    <row r="51" spans="1:10" ht="45.75" customHeight="1" thickBot="1">
+      <c r="A51" s="15"/>
+      <c r="B51" s="68"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="18"/>
+      <c r="G51" s="18"/>
+      <c r="H51" s="89"/>
+      <c r="I51" s="92"/>
+      <c r="J51" s="81"/>
+    </row>
+    <row r="52" spans="1:10" ht="6.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A52" s="15"/>
+      <c r="B52" s="28"/>
+      <c r="C52" s="35"/>
+      <c r="D52" s="33"/>
+      <c r="E52" s="34"/>
+      <c r="F52" s="39"/>
+      <c r="G52" s="35"/>
+      <c r="H52" s="36"/>
+      <c r="I52" s="52"/>
+      <c r="J52" s="52"/>
+    </row>
+    <row r="53" spans="1:10" ht="45" customHeight="1" thickTop="1">
+      <c r="A53" s="15"/>
+      <c r="B53" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="C53" s="13"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="86"/>
+      <c r="I53" s="93" t="s">
+        <v>68</v>
+      </c>
+      <c r="J53" s="80"/>
+    </row>
+    <row r="54" spans="1:10" ht="45.75" customHeight="1">
+      <c r="B54" s="58"/>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
-      <c r="E54" s="10"/>
-      <c r="F54" s="10"/>
+      <c r="E54" s="8"/>
+      <c r="F54" s="8"/>
       <c r="G54" s="4"/>
-      <c r="H54" s="12"/>
-    </row>
-    <row r="55" spans="1:8" ht="45" customHeight="1">
-      <c r="B55" s="66"/>
+      <c r="H54" s="3"/>
+      <c r="I54" s="91"/>
+      <c r="J54" s="81"/>
+    </row>
+    <row r="55" spans="1:10" ht="45" customHeight="1">
+      <c r="B55" s="58"/>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
       <c r="E55" s="3"/>
-      <c r="F55" s="10"/>
+      <c r="F55" s="8"/>
       <c r="G55" s="4"/>
-      <c r="H55" s="12"/>
-    </row>
-    <row r="56" spans="1:8" ht="44.25" customHeight="1" thickBot="1">
-      <c r="B56" s="67"/>
-      <c r="C56" s="23"/>
-      <c r="D56" s="23"/>
-      <c r="E56" s="24"/>
-      <c r="F56" s="23"/>
-      <c r="G56" s="23"/>
-      <c r="H56" s="25"/>
-    </row>
-    <row r="57" spans="1:8" ht="15" thickTop="1">
+      <c r="H55" s="3"/>
+      <c r="I55" s="91"/>
+      <c r="J55" s="81"/>
+    </row>
+    <row r="56" spans="1:10" ht="44.25" customHeight="1" thickBot="1">
+      <c r="B56" s="59"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="19"/>
+      <c r="F56" s="18"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="19"/>
+      <c r="I56" s="94"/>
+      <c r="J56" s="82"/>
+    </row>
+    <row r="57" spans="1:10" ht="15" thickTop="1">
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:10">
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:10">
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:10">
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:10">
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:10">
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="20">
+    <mergeCell ref="I48:I51"/>
+    <mergeCell ref="J48:J51"/>
+    <mergeCell ref="I53:I56"/>
+    <mergeCell ref="J53:J56"/>
+    <mergeCell ref="I17:I20"/>
+    <mergeCell ref="J17:J20"/>
+    <mergeCell ref="I22:I29"/>
+    <mergeCell ref="J22:J29"/>
+    <mergeCell ref="I31:I45"/>
+    <mergeCell ref="J31:J45"/>
     <mergeCell ref="B53:B56"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B17:B20"/>
@@ -2520,18 +2740,17 @@
     <mergeCell ref="B48:B51"/>
     <mergeCell ref="B31:B45"/>
     <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:E6"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
-  <conditionalFormatting sqref="C33:E45 G32:H45 C32:D32 H22:H31">
+  <conditionalFormatting sqref="C33:E45 G32:H45 C32:D32 H22:J22 H30:J31 H23:H29">
     <cfRule type="expression" dxfId="20" priority="24" stopIfTrue="1">
       <formula>$H22="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E22:E32 C22:D31 G22:G31 C17:H17 C19:H21 C18:E18 G18:H18">
+  <conditionalFormatting sqref="E22:E32 C22:D31 G22:G31 C17:J17 C21:J21 C18:E18 G18:H18 C19:H20">
     <cfRule type="expression" dxfId="19" priority="29" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
@@ -2551,7 +2770,7 @@
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50:E51 G49:H51 C49:D49 H48">
+  <conditionalFormatting sqref="C50:E51 G49:H51 C49:D49 H48:J48">
     <cfRule type="expression" dxfId="15" priority="15" stopIfTrue="1">
       <formula>$H48="close"</formula>
     </cfRule>
@@ -2576,7 +2795,7 @@
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H46:H47">
+  <conditionalFormatting sqref="H46:J47">
     <cfRule type="expression" dxfId="10" priority="10" stopIfTrue="1">
       <formula>$H46="close"</formula>
     </cfRule>
@@ -2591,7 +2810,7 @@
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H52">
+  <conditionalFormatting sqref="H52:J52">
     <cfRule type="expression" dxfId="7" priority="7" stopIfTrue="1">
       <formula>$H52="close"</formula>
     </cfRule>
@@ -2606,7 +2825,7 @@
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C55:E56 G54:H56 C54:D54 H53">
+  <conditionalFormatting sqref="C55:E56 G54:H56 C54:D54 H53:J53">
     <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
       <formula>$H53="close"</formula>
     </cfRule>
@@ -2631,7 +2850,7 @@
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F56 F51">
       <formula1>"Organizational,Technical, Business ,Product"</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
Add review on GUI
</commit_message>
<xml_diff>
--- a/Design/Design document Peer Review sheet.xlsx
+++ b/Design/Design document Peer Review sheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed\Documents\GitHub\Internet-Banking-System\Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\Internet-Banking-System\Internet-Banking-System\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3600" windowWidth="20490" windowHeight="7890"/>
+    <workbookView xWindow="0" yWindow="3600" windowWidth="20496" windowHeight="7896"/>
   </bookViews>
   <sheets>
     <sheet name="SRS-PR Sheet" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="91">
   <si>
     <t>Priority</t>
   </si>
@@ -262,6 +262,71 @@
   </si>
   <si>
     <t>Update peer review sheet</t>
+  </si>
+  <si>
+    <t>Bank_SYS_DSN_001,
+Bank_SYS_DSN_002,
+Bank_SYS_DSN_003,
+Bank_SYS_DSN_010,
+Bank_SYS_DSN_011,
+Bank_SYS_DSN_012,
+Bank_SYS_DSN_013,
+Bank_SYS_DSN_015</t>
+  </si>
+  <si>
+    <t>fields constrains must be written beside the fields in the wireframe</t>
+  </si>
+  <si>
+    <t>missing screen when user enters wrong verification code</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Reg_R026</t>
+  </si>
+  <si>
+    <t>Admin page wireframe should contain Admin user name not customer user name</t>
+  </si>
+  <si>
+    <t>Bank_SYS_DSN_015</t>
+  </si>
+  <si>
+    <t>missing screen of previous transactions error message when user doesn't have transactions in the requested period</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_PT_R015</t>
+  </si>
+  <si>
+    <t>Bank_SYS_DSN_011</t>
+  </si>
+  <si>
+    <t>wrong error message when user exceeds the amount. It should be "You have exceeded the amount of money allowed to be transferred"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BANK_SYS_SRS_TR_R027 </t>
+  </si>
+  <si>
+    <t>wrong message text when user enters wrong account id. It should be "You have entered an invalid account , Please try again"</t>
+  </si>
+  <si>
+    <t>Bank_SYS_DSN_012</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_TR_R007</t>
+  </si>
+  <si>
+    <t>wrong message text when user enters amount greater than his balance. It should be "you don't have the required amount , please check your balance"</t>
+  </si>
+  <si>
+    <t>Bank_SYS_DSN_013</t>
+  </si>
+  <si>
+    <t>unclear coloring of amount in listing page, should be explained by modifying "from account id" and "to account id"</t>
+  </si>
+  <si>
+    <t>Bank_SYS_DSN_014</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_PT_R021,
+BANK_SYS_SRS_PT_R022</t>
   </si>
 </sst>
 </file>
@@ -955,7 +1020,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1190,6 +1255,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1205,7 +1282,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1283,15 +1360,64 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="標準_REQM_20100521" xfId="1"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="28">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1884,36 +2010,36 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J62"/>
+  <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A47" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="5.75" style="2" customWidth="1"/>
-    <col min="2" max="2" width="20.125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="27.375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="36.75" style="5" customWidth="1"/>
-    <col min="5" max="5" width="54.5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="27.875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="18.125" style="2" customWidth="1"/>
-    <col min="8" max="10" width="39.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="5.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="20.109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="36.77734375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="54.44140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="27.88671875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="18.109375" style="2" customWidth="1"/>
+    <col min="8" max="10" width="39.88671875" style="2" customWidth="1"/>
     <col min="11" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1"/>
+    <row r="1" spans="1:10" ht="14.4" thickBot="1"/>
     <row r="2" spans="1:10" ht="105" customHeight="1" thickBot="1">
-      <c r="B2" s="94" t="s">
+      <c r="B2" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="96"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="100"/>
       <c r="I2" s="69"/>
       <c r="J2" s="69"/>
     </row>
@@ -1932,25 +2058,25 @@
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:10" ht="20.25" customHeight="1">
-      <c r="C5" s="105" t="s">
+      <c r="C5" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="105" t="s">
+      <c r="D5" s="109" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="107" t="s">
+      <c r="E5" s="111" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="103" t="s">
+      <c r="F5" s="107" t="s">
         <v>69</v>
       </c>
-      <c r="G5" s="109"/>
+      <c r="G5" s="79"/>
     </row>
     <row r="6" spans="1:10" ht="23.25" customHeight="1" thickBot="1">
-      <c r="C6" s="106"/>
-      <c r="D6" s="106"/>
-      <c r="E6" s="108"/>
-      <c r="F6" s="104"/>
+      <c r="C6" s="110"/>
+      <c r="D6" s="110"/>
+      <c r="E6" s="112"/>
+      <c r="F6" s="108"/>
       <c r="G6" s="70"/>
     </row>
     <row r="7" spans="1:10" ht="29.25" customHeight="1">
@@ -2074,7 +2200,7 @@
     </row>
     <row r="17" spans="1:10" ht="139.5" customHeight="1" thickTop="1">
       <c r="A17" s="15"/>
-      <c r="B17" s="97" t="s">
+      <c r="B17" s="101" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="13" t="s">
@@ -2095,16 +2221,16 @@
       <c r="H17" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="I17" s="85" t="s">
+      <c r="I17" s="89" t="s">
         <v>65</v>
       </c>
-      <c r="J17" s="86">
+      <c r="J17" s="90">
         <v>43743</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="57" customHeight="1" thickBot="1">
       <c r="A18" s="15"/>
-      <c r="B18" s="92"/>
+      <c r="B18" s="96"/>
       <c r="C18" s="4" t="s">
         <v>20</v>
       </c>
@@ -2121,12 +2247,12 @@
         <v>23</v>
       </c>
       <c r="H18" s="3"/>
-      <c r="I18" s="85"/>
-      <c r="J18" s="87"/>
+      <c r="I18" s="89"/>
+      <c r="J18" s="91"/>
     </row>
     <row r="19" spans="1:10" ht="54.75" customHeight="1">
       <c r="A19" s="15"/>
-      <c r="B19" s="92"/>
+      <c r="B19" s="96"/>
       <c r="C19" s="4" t="s">
         <v>21</v>
       </c>
@@ -2143,12 +2269,12 @@
         <v>23</v>
       </c>
       <c r="H19" s="3"/>
-      <c r="I19" s="85"/>
-      <c r="J19" s="87"/>
+      <c r="I19" s="89"/>
+      <c r="J19" s="91"/>
     </row>
     <row r="20" spans="1:10" s="1" customFormat="1" ht="72.75" customHeight="1" thickBot="1">
       <c r="A20" s="16"/>
-      <c r="B20" s="98"/>
+      <c r="B20" s="102"/>
       <c r="C20" s="26" t="s">
         <v>22</v>
       </c>
@@ -2165,8 +2291,8 @@
         <v>23</v>
       </c>
       <c r="H20" s="19"/>
-      <c r="I20" s="85"/>
-      <c r="J20" s="87"/>
+      <c r="I20" s="89"/>
+      <c r="J20" s="91"/>
     </row>
     <row r="21" spans="1:10" s="6" customFormat="1" ht="4.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A21" s="17"/>
@@ -2182,7 +2308,7 @@
     </row>
     <row r="22" spans="1:10" ht="57" customHeight="1" thickTop="1">
       <c r="A22" s="15"/>
-      <c r="B22" s="99" t="s">
+      <c r="B22" s="103" t="s">
         <v>13</v>
       </c>
       <c r="C22" s="13"/>
@@ -2193,94 +2319,96 @@
       <c r="F22" s="14"/>
       <c r="G22" s="13"/>
       <c r="H22" s="30"/>
-      <c r="I22" s="88" t="s">
+      <c r="I22" s="92" t="s">
         <v>66</v>
       </c>
-      <c r="J22" s="89"/>
+      <c r="J22" s="93">
+        <v>43743</v>
+      </c>
     </row>
     <row r="23" spans="1:10" ht="54.75" customHeight="1">
       <c r="A23" s="15"/>
-      <c r="B23" s="100"/>
+      <c r="B23" s="104"/>
       <c r="C23" s="4"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
-      <c r="I23" s="88"/>
-      <c r="J23" s="90"/>
+      <c r="I23" s="92"/>
+      <c r="J23" s="94"/>
     </row>
     <row r="24" spans="1:10" ht="60" customHeight="1">
       <c r="A24" s="15"/>
-      <c r="B24" s="100"/>
+      <c r="B24" s="104"/>
       <c r="C24" s="4"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
-      <c r="I24" s="88"/>
-      <c r="J24" s="90"/>
+      <c r="I24" s="92"/>
+      <c r="J24" s="94"/>
     </row>
     <row r="25" spans="1:10" ht="60" customHeight="1">
       <c r="A25" s="15"/>
-      <c r="B25" s="100"/>
+      <c r="B25" s="104"/>
       <c r="C25" s="26"/>
       <c r="D25" s="32"/>
       <c r="E25" s="32"/>
       <c r="F25" s="32"/>
       <c r="G25" s="26"/>
       <c r="H25" s="26"/>
-      <c r="I25" s="88"/>
-      <c r="J25" s="90"/>
+      <c r="I25" s="92"/>
+      <c r="J25" s="94"/>
     </row>
     <row r="26" spans="1:10" ht="60" customHeight="1">
       <c r="A26" s="15"/>
-      <c r="B26" s="100"/>
+      <c r="B26" s="104"/>
       <c r="C26" s="26"/>
       <c r="D26" s="32"/>
       <c r="E26" s="32"/>
       <c r="F26" s="32"/>
       <c r="G26" s="26"/>
       <c r="H26" s="26"/>
-      <c r="I26" s="88"/>
-      <c r="J26" s="90"/>
+      <c r="I26" s="92"/>
+      <c r="J26" s="94"/>
     </row>
     <row r="27" spans="1:10" ht="60" customHeight="1">
       <c r="A27" s="15"/>
-      <c r="B27" s="100"/>
+      <c r="B27" s="104"/>
       <c r="C27" s="26"/>
       <c r="D27" s="32"/>
       <c r="E27" s="32"/>
       <c r="F27" s="32"/>
       <c r="G27" s="26"/>
       <c r="H27" s="26"/>
-      <c r="I27" s="88"/>
-      <c r="J27" s="90"/>
+      <c r="I27" s="92"/>
+      <c r="J27" s="94"/>
     </row>
     <row r="28" spans="1:10" ht="60" customHeight="1">
       <c r="A28" s="15"/>
-      <c r="B28" s="100"/>
+      <c r="B28" s="104"/>
       <c r="C28" s="26"/>
       <c r="D28" s="32"/>
       <c r="E28" s="32"/>
       <c r="F28" s="32"/>
       <c r="G28" s="26"/>
       <c r="H28" s="26"/>
-      <c r="I28" s="88"/>
-      <c r="J28" s="90"/>
+      <c r="I28" s="92"/>
+      <c r="J28" s="94"/>
     </row>
     <row r="29" spans="1:10" ht="51.75" customHeight="1" thickBot="1">
       <c r="A29" s="15"/>
-      <c r="B29" s="101"/>
+      <c r="B29" s="105"/>
       <c r="C29" s="26"/>
       <c r="D29" s="32"/>
       <c r="E29" s="32"/>
       <c r="F29" s="32"/>
       <c r="G29" s="26"/>
       <c r="H29" s="18"/>
-      <c r="I29" s="88"/>
-      <c r="J29" s="90"/>
+      <c r="I29" s="92"/>
+      <c r="J29" s="94"/>
     </row>
     <row r="30" spans="1:10" ht="5.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A30" s="15"/>
@@ -2296,7 +2424,7 @@
     </row>
     <row r="31" spans="1:10" ht="71.25" customHeight="1" thickTop="1">
       <c r="A31" s="15"/>
-      <c r="B31" s="92" t="s">
+      <c r="B31" s="96" t="s">
         <v>14</v>
       </c>
       <c r="C31" s="13"/>
@@ -2313,16 +2441,16 @@
         <v>23</v>
       </c>
       <c r="H31" s="65"/>
-      <c r="I31" s="88" t="s">
+      <c r="I31" s="92" t="s">
         <v>67</v>
       </c>
-      <c r="J31" s="89">
+      <c r="J31" s="93">
         <v>43743</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="63" customHeight="1">
       <c r="A32" s="15"/>
-      <c r="B32" s="92"/>
+      <c r="B32" s="96"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4" t="s">
         <v>37</v>
@@ -2337,12 +2465,12 @@
         <v>40</v>
       </c>
       <c r="H32" s="3"/>
-      <c r="I32" s="88"/>
-      <c r="J32" s="90"/>
+      <c r="I32" s="92"/>
+      <c r="J32" s="94"/>
     </row>
     <row r="33" spans="1:10" ht="62.25" customHeight="1">
       <c r="A33" s="15"/>
-      <c r="B33" s="92"/>
+      <c r="B33" s="96"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4" t="s">
         <v>53</v>
@@ -2357,12 +2485,12 @@
         <v>23</v>
       </c>
       <c r="H33" s="3"/>
-      <c r="I33" s="88"/>
-      <c r="J33" s="90"/>
+      <c r="I33" s="92"/>
+      <c r="J33" s="94"/>
     </row>
     <row r="34" spans="1:10" ht="62.25" customHeight="1">
       <c r="A34" s="15"/>
-      <c r="B34" s="92"/>
+      <c r="B34" s="96"/>
       <c r="C34" s="26"/>
       <c r="D34" s="26" t="s">
         <v>41</v>
@@ -2375,12 +2503,12 @@
         <v>23</v>
       </c>
       <c r="H34" s="27"/>
-      <c r="I34" s="88"/>
-      <c r="J34" s="90"/>
+      <c r="I34" s="92"/>
+      <c r="J34" s="94"/>
     </row>
     <row r="35" spans="1:10" ht="62.25" customHeight="1">
       <c r="A35" s="15"/>
-      <c r="B35" s="92"/>
+      <c r="B35" s="96"/>
       <c r="C35" s="26"/>
       <c r="D35" s="26" t="s">
         <v>45</v>
@@ -2395,12 +2523,12 @@
         <v>23</v>
       </c>
       <c r="H35" s="27"/>
-      <c r="I35" s="88"/>
-      <c r="J35" s="90"/>
+      <c r="I35" s="92"/>
+      <c r="J35" s="94"/>
     </row>
     <row r="36" spans="1:10" ht="62.25" customHeight="1">
       <c r="A36" s="15"/>
-      <c r="B36" s="92"/>
+      <c r="B36" s="96"/>
       <c r="C36" s="26"/>
       <c r="D36" s="26" t="s">
         <v>48</v>
@@ -2415,12 +2543,12 @@
         <v>23</v>
       </c>
       <c r="H36" s="27"/>
-      <c r="I36" s="88"/>
-      <c r="J36" s="90"/>
+      <c r="I36" s="92"/>
+      <c r="J36" s="94"/>
     </row>
     <row r="37" spans="1:10" ht="62.25" customHeight="1">
       <c r="A37" s="15"/>
-      <c r="B37" s="92"/>
+      <c r="B37" s="96"/>
       <c r="C37" s="26"/>
       <c r="D37" s="26" t="s">
         <v>49</v>
@@ -2435,12 +2563,12 @@
         <v>52</v>
       </c>
       <c r="H37" s="27"/>
-      <c r="I37" s="88"/>
-      <c r="J37" s="90"/>
+      <c r="I37" s="92"/>
+      <c r="J37" s="94"/>
     </row>
     <row r="38" spans="1:10" ht="62.25" customHeight="1">
       <c r="A38" s="15"/>
-      <c r="B38" s="92"/>
+      <c r="B38" s="96"/>
       <c r="C38" s="26"/>
       <c r="D38" s="26" t="s">
         <v>55</v>
@@ -2455,12 +2583,12 @@
         <v>23</v>
       </c>
       <c r="H38" s="27"/>
-      <c r="I38" s="88"/>
-      <c r="J38" s="90"/>
+      <c r="I38" s="92"/>
+      <c r="J38" s="94"/>
     </row>
     <row r="39" spans="1:10" ht="62.25" customHeight="1">
       <c r="A39" s="15"/>
-      <c r="B39" s="92"/>
+      <c r="B39" s="96"/>
       <c r="C39" s="26"/>
       <c r="D39" s="26" t="s">
         <v>55</v>
@@ -2475,12 +2603,12 @@
         <v>23</v>
       </c>
       <c r="H39" s="27"/>
-      <c r="I39" s="88"/>
-      <c r="J39" s="90"/>
+      <c r="I39" s="92"/>
+      <c r="J39" s="94"/>
     </row>
     <row r="40" spans="1:10" ht="62.25" customHeight="1">
       <c r="A40" s="15"/>
-      <c r="B40" s="92"/>
+      <c r="B40" s="96"/>
       <c r="C40" s="26"/>
       <c r="D40" s="26" t="s">
         <v>60</v>
@@ -2495,12 +2623,12 @@
         <v>23</v>
       </c>
       <c r="H40" s="27"/>
-      <c r="I40" s="88"/>
-      <c r="J40" s="90"/>
+      <c r="I40" s="92"/>
+      <c r="J40" s="94"/>
     </row>
     <row r="41" spans="1:10" ht="62.25" customHeight="1">
       <c r="A41" s="15"/>
-      <c r="B41" s="92"/>
+      <c r="B41" s="96"/>
       <c r="C41" s="26"/>
       <c r="D41" s="26" t="s">
         <v>62</v>
@@ -2515,12 +2643,12 @@
         <v>40</v>
       </c>
       <c r="H41" s="27"/>
-      <c r="I41" s="88"/>
-      <c r="J41" s="90"/>
+      <c r="I41" s="92"/>
+      <c r="J41" s="94"/>
     </row>
     <row r="42" spans="1:10" ht="62.25" customHeight="1">
       <c r="A42" s="15"/>
-      <c r="B42" s="92"/>
+      <c r="B42" s="96"/>
       <c r="C42" s="26"/>
       <c r="D42" s="26" t="s">
         <v>63</v>
@@ -2533,44 +2661,44 @@
         <v>23</v>
       </c>
       <c r="H42" s="27"/>
-      <c r="I42" s="88"/>
-      <c r="J42" s="90"/>
+      <c r="I42" s="92"/>
+      <c r="J42" s="94"/>
     </row>
     <row r="43" spans="1:10" ht="62.25" customHeight="1">
       <c r="A43" s="15"/>
-      <c r="B43" s="92"/>
+      <c r="B43" s="96"/>
       <c r="C43" s="26"/>
       <c r="D43" s="26"/>
       <c r="E43" s="55"/>
       <c r="F43" s="32"/>
       <c r="G43" s="26"/>
       <c r="H43" s="27"/>
-      <c r="I43" s="88"/>
-      <c r="J43" s="90"/>
+      <c r="I43" s="92"/>
+      <c r="J43" s="94"/>
     </row>
     <row r="44" spans="1:10" ht="62.25" customHeight="1">
       <c r="A44" s="15"/>
-      <c r="B44" s="92"/>
+      <c r="B44" s="96"/>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
       <c r="E44" s="55"/>
       <c r="F44" s="32"/>
       <c r="G44" s="26"/>
       <c r="H44" s="27"/>
-      <c r="I44" s="88"/>
-      <c r="J44" s="90"/>
+      <c r="I44" s="92"/>
+      <c r="J44" s="94"/>
     </row>
     <row r="45" spans="1:10" ht="62.25" customHeight="1" thickBot="1">
       <c r="A45" s="15"/>
-      <c r="B45" s="92"/>
+      <c r="B45" s="96"/>
       <c r="C45" s="26"/>
       <c r="D45" s="26"/>
       <c r="E45" s="55"/>
       <c r="F45" s="32"/>
       <c r="G45" s="26"/>
       <c r="H45" s="19"/>
-      <c r="I45" s="88"/>
-      <c r="J45" s="90"/>
+      <c r="I45" s="92"/>
+      <c r="J45" s="94"/>
     </row>
     <row r="46" spans="1:10" ht="6.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A46" s="15"/>
@@ -2597,7 +2725,7 @@
       <c r="J47" s="54"/>
     </row>
     <row r="48" spans="1:10" ht="58.5" customHeight="1">
-      <c r="B48" s="92" t="s">
+      <c r="B48" s="96" t="s">
         <v>15</v>
       </c>
       <c r="C48" s="13"/>
@@ -2606,44 +2734,44 @@
       <c r="F48" s="14"/>
       <c r="G48" s="13"/>
       <c r="H48" s="66"/>
-      <c r="I48" s="77" t="s">
+      <c r="I48" s="81" t="s">
         <v>67</v>
       </c>
-      <c r="J48" s="80"/>
+      <c r="J48" s="84"/>
     </row>
     <row r="49" spans="1:10" ht="48.75" customHeight="1">
-      <c r="B49" s="92"/>
+      <c r="B49" s="96"/>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
       <c r="E49" s="8"/>
       <c r="F49" s="8"/>
       <c r="G49" s="4"/>
       <c r="H49" s="67"/>
-      <c r="I49" s="78"/>
-      <c r="J49" s="80"/>
+      <c r="I49" s="82"/>
+      <c r="J49" s="84"/>
     </row>
     <row r="50" spans="1:10" ht="51.75" customHeight="1">
-      <c r="B50" s="92"/>
+      <c r="B50" s="96"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
       <c r="E50" s="3"/>
       <c r="F50" s="8"/>
       <c r="G50" s="4"/>
       <c r="H50" s="67"/>
-      <c r="I50" s="78"/>
-      <c r="J50" s="80"/>
+      <c r="I50" s="82"/>
+      <c r="J50" s="84"/>
     </row>
     <row r="51" spans="1:10" ht="45.75" customHeight="1" thickBot="1">
       <c r="A51" s="15"/>
-      <c r="B51" s="102"/>
+      <c r="B51" s="106"/>
       <c r="C51" s="18"/>
       <c r="D51" s="18"/>
       <c r="E51" s="19"/>
       <c r="F51" s="18"/>
       <c r="G51" s="18"/>
       <c r="H51" s="68"/>
-      <c r="I51" s="79"/>
-      <c r="J51" s="80"/>
+      <c r="I51" s="83"/>
+      <c r="J51" s="84"/>
     </row>
     <row r="52" spans="1:10" ht="6.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A52" s="15"/>
@@ -2657,72 +2785,163 @@
       <c r="I52" s="52"/>
       <c r="J52" s="52"/>
     </row>
-    <row r="53" spans="1:10" ht="45" customHeight="1" thickTop="1">
+    <row r="53" spans="1:10" ht="137.4" customHeight="1" thickTop="1">
       <c r="A53" s="15"/>
-      <c r="B53" s="91" t="s">
+      <c r="B53" s="95" t="s">
         <v>16</v>
       </c>
       <c r="C53" s="13"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
+      <c r="D53" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E53" s="14" t="s">
+        <v>73</v>
+      </c>
       <c r="F53" s="14"/>
-      <c r="G53" s="13"/>
+      <c r="G53" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="H53" s="65"/>
-      <c r="I53" s="81" t="s">
+      <c r="I53" s="85" t="s">
         <v>68</v>
       </c>
-      <c r="J53" s="83"/>
-    </row>
-    <row r="54" spans="1:10" ht="45.75" customHeight="1">
-      <c r="B54" s="92"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="4"/>
-      <c r="E54" s="8"/>
-      <c r="F54" s="8"/>
-      <c r="G54" s="4"/>
-      <c r="H54" s="3"/>
-      <c r="I54" s="78"/>
-      <c r="J54" s="80"/>
-    </row>
-    <row r="55" spans="1:10" ht="45" customHeight="1">
-      <c r="B55" s="92"/>
+      <c r="J53" s="87">
+        <v>43743</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="45" customHeight="1">
+      <c r="A54" s="50"/>
+      <c r="B54" s="95"/>
+      <c r="C54" s="78"/>
+      <c r="D54" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E54" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="F54" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="G54" s="78" t="s">
+        <v>23</v>
+      </c>
+      <c r="H54" s="80"/>
+      <c r="I54" s="82"/>
+      <c r="J54" s="84"/>
+    </row>
+    <row r="55" spans="1:10" ht="45.75" customHeight="1">
+      <c r="B55" s="96"/>
       <c r="C55" s="4"/>
-      <c r="D55" s="4"/>
-      <c r="E55" s="3"/>
+      <c r="D55" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>76</v>
+      </c>
       <c r="F55" s="8"/>
-      <c r="G55" s="4"/>
+      <c r="G55" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="H55" s="3"/>
-      <c r="I55" s="78"/>
-      <c r="J55" s="80"/>
-    </row>
-    <row r="56" spans="1:10" ht="44.25" customHeight="1" thickBot="1">
-      <c r="B56" s="93"/>
-      <c r="C56" s="18"/>
-      <c r="D56" s="18"/>
-      <c r="E56" s="19"/>
-      <c r="F56" s="18"/>
-      <c r="G56" s="18"/>
-      <c r="H56" s="19"/>
+      <c r="I55" s="82"/>
+      <c r="J55" s="84"/>
+    </row>
+    <row r="56" spans="1:10" ht="45.75" customHeight="1">
+      <c r="B56" s="96"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="F56" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G56" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H56" s="3"/>
       <c r="I56" s="82"/>
       <c r="J56" s="84"/>
     </row>
-    <row r="57" spans="1:10" ht="15" thickTop="1">
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
-    </row>
-    <row r="58" spans="1:10">
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
-    </row>
-    <row r="59" spans="1:10">
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
-    </row>
-    <row r="60" spans="1:10">
-      <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
-    </row>
-    <row r="61" spans="1:10">
+    <row r="57" spans="1:10" ht="45" customHeight="1">
+      <c r="B57" s="96"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E57" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F57" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H57" s="3"/>
+      <c r="I57" s="82"/>
+      <c r="J57" s="84"/>
+    </row>
+    <row r="58" spans="1:10" ht="45" customHeight="1">
+      <c r="B58" s="96"/>
+      <c r="C58" s="77"/>
+      <c r="D58" s="77" t="s">
+        <v>84</v>
+      </c>
+      <c r="E58" s="55" t="s">
+        <v>83</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="G58" s="77" t="s">
+        <v>40</v>
+      </c>
+      <c r="H58" s="27"/>
+      <c r="I58" s="82"/>
+      <c r="J58" s="84"/>
+    </row>
+    <row r="59" spans="1:10" ht="45" customHeight="1">
+      <c r="B59" s="96"/>
+      <c r="C59" s="77"/>
+      <c r="D59" s="77" t="s">
+        <v>87</v>
+      </c>
+      <c r="E59" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="F59" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G59" s="77" t="s">
+        <v>40</v>
+      </c>
+      <c r="H59" s="27"/>
+      <c r="I59" s="82"/>
+      <c r="J59" s="84"/>
+    </row>
+    <row r="60" spans="1:10" ht="44.25" customHeight="1" thickBot="1">
+      <c r="B60" s="97"/>
+      <c r="C60" s="18"/>
+      <c r="D60" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="E60" s="113" t="s">
+        <v>88</v>
+      </c>
+      <c r="F60" s="113" t="s">
+        <v>90</v>
+      </c>
+      <c r="G60" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="H60" s="19"/>
+      <c r="I60" s="86"/>
+      <c r="J60" s="88"/>
+    </row>
+    <row r="61" spans="1:10" ht="14.4" thickTop="1">
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
     </row>
@@ -2730,9 +2949,25 @@
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
     </row>
+    <row r="63" spans="1:10">
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+    </row>
+    <row r="65" spans="3:4">
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+    </row>
+    <row r="66" spans="3:4">
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B53:B56"/>
+    <mergeCell ref="B53:B60"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B17:B20"/>
     <mergeCell ref="B22:B29"/>
@@ -2744,8 +2979,8 @@
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="I48:I51"/>
     <mergeCell ref="J48:J51"/>
-    <mergeCell ref="I53:I56"/>
-    <mergeCell ref="J53:J56"/>
+    <mergeCell ref="I53:I60"/>
+    <mergeCell ref="J53:J60"/>
     <mergeCell ref="I17:I20"/>
     <mergeCell ref="J17:J20"/>
     <mergeCell ref="I22:I29"/>
@@ -2754,116 +2989,136 @@
     <mergeCell ref="J31:J45"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
-  <conditionalFormatting sqref="C33:E45 G32:H45 C32:D32 H22:J22 H30:J31 H23:H29">
-    <cfRule type="expression" dxfId="20" priority="24" stopIfTrue="1">
+  <conditionalFormatting sqref="C33:E45 G32:H45 C32:D32 H22:J22 H30:J31 H23:H29 C60:E60 C59:D59">
+    <cfRule type="expression" dxfId="27" priority="28" stopIfTrue="1">
       <formula>$H22="close"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22:E32 C22:D31 G22:G31 C17:J17 C21:J21 C18:E18 G18:H18 C19:H20">
-    <cfRule type="expression" dxfId="19" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="33" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22:F29 F32:F45">
-    <cfRule type="expression" dxfId="18" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="23" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F30">
-    <cfRule type="expression" dxfId="17" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="22" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F31">
-    <cfRule type="expression" dxfId="16" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="21" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50:E51 G49:H51 C49:D49 H48:J48">
-    <cfRule type="expression" dxfId="15" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="19" stopIfTrue="1">
       <formula>$H48="close"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F51">
-    <cfRule type="expression" dxfId="14" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="18" stopIfTrue="1">
       <formula>$H51="close"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E48:E49 C48:D48 G48">
-    <cfRule type="expression" dxfId="13" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="20" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F49:F50">
-    <cfRule type="expression" dxfId="12" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="17" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F48">
-    <cfRule type="expression" dxfId="11" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="16" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H46:J47">
-    <cfRule type="expression" dxfId="10" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="14" stopIfTrue="1">
       <formula>$H46="close"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:E47 G46:G47">
-    <cfRule type="expression" dxfId="9" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="15" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F46:F47">
-    <cfRule type="expression" dxfId="8" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="13" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H52:J52">
-    <cfRule type="expression" dxfId="7" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="11" stopIfTrue="1">
       <formula>$H52="close"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52:E52 G52">
-    <cfRule type="expression" dxfId="6" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="12" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F52">
-    <cfRule type="expression" dxfId="5" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="10" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C55:E56 G54:H56 C54:D54 H53:J53">
-    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
+  <conditionalFormatting sqref="C57:E57 G55:H60 C55:D56 H53:J54 C58:D58">
+    <cfRule type="expression" dxfId="11" priority="8" stopIfTrue="1">
       <formula>$H53="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F56">
-    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
-      <formula>$H56="close"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E53:E54 C53:D53 G53">
-    <cfRule type="expression" dxfId="2" priority="5" stopIfTrue="1">
+  <conditionalFormatting sqref="E53:E56 C54:D54 G53:G54 C53">
+    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F54:F55">
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+  <conditionalFormatting sqref="F55:F57">
+    <cfRule type="expression" dxfId="8" priority="6" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F53">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+  <conditionalFormatting sqref="F53:F54">
+    <cfRule type="expression" dxfId="7" priority="5" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F56 F51">
+  <conditionalFormatting sqref="E58">
+    <cfRule type="expression" dxfId="6" priority="35" stopIfTrue="1">
+      <formula>$H59="close"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E59">
+    <cfRule type="expression" dxfId="5" priority="4" stopIfTrue="1">
+      <formula>$H59="close"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F58:F59">
+    <cfRule type="expression" dxfId="4" priority="3" stopIfTrue="1">
+      <formula>#REF!="close"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F60">
+    <cfRule type="expression" dxfId="3" priority="2" stopIfTrue="1">
+      <formula>$H60="close"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D53">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+      <formula>#REF!="close"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F51">
       <formula1>"Organizational,Technical, Business ,Product"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H22:H56">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H22:H60">
       <formula1>"close,open"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update Design Document Peer Review
Reviewing DD/Class Diagram
</commit_message>
<xml_diff>
--- a/Design/Design document Peer Review sheet.xlsx
+++ b/Design/Design document Peer Review sheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\Internet-Banking-System\Internet-Banking-System\Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Internet-Banking-System\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3600" windowWidth="20496" windowHeight="7896"/>
+    <workbookView xWindow="0" yWindow="3600" windowWidth="20490" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="SRS-PR Sheet" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="120">
   <si>
     <t>Priority</t>
   </si>
@@ -71,31 +71,13 @@
     <t>Detailed Design</t>
   </si>
   <si>
-    <t>Data Flow Diagram</t>
-  </si>
-  <si>
-    <t>Data Model ERD</t>
-  </si>
-  <si>
     <t>GUI</t>
   </si>
   <si>
     <t xml:space="preserve"> Date</t>
   </si>
   <si>
-    <t>1-</t>
-  </si>
-  <si>
     <t>missing in( C)(2) to check balance before transferring money to an account in the same bank</t>
-  </si>
-  <si>
-    <t>2-</t>
-  </si>
-  <si>
-    <t>3-</t>
-  </si>
-  <si>
-    <t>4-</t>
   </si>
   <si>
     <t>High</t>
@@ -164,10 +146,6 @@
   </si>
   <si>
     <t>Bank_Sys_DM_ADMIN_004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-</t>
   </si>
   <si>
     <t>1-when admin login or register sucessfully he will be redirected to admin home page not customer page
@@ -328,11 +306,120 @@
     <t>BANK_SYS_SRS_PT_R021,
 BANK_SYS_SRS_PT_R022</t>
   </si>
+  <si>
+    <t>Missing relation between transaction and previous transaction ,it should be a composition as we discussed</t>
+  </si>
+  <si>
+    <t>Detailed Design Class Diagram Document Version 1.1</t>
+  </si>
+  <si>
+    <t>Unclear Relation between "Previous Transaction" and Account , it should be between "Transactions " and "Previous Transactions"</t>
+  </si>
+  <si>
+    <t>Relationship between "Account" and "Transactions" is one to one , it should be one to many based on the same logic we used in ERD.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unclear Relation between " Admin" and "Client" </t>
+  </si>
+  <si>
+    <t>The Relationship between can be 1 to 1 based on the emplementaion of the syatem but in this case we would have conflict between ERD document and Class Diagram Document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&lt;use&gt;&gt; between admin and Client is unclear we may assume it's something like the relation between Bank and Client like in this link https://creately.com/diagram/example/ihww1rk21/online%20banking%20system
+</t>
+  </si>
+  <si>
+    <t>Data Model</t>
+  </si>
+  <si>
+    <t>Bank_Sys_Design_GUI_Issue_001</t>
+  </si>
+  <si>
+    <t>Bank_Sys_Design_GUI_Issue_002</t>
+  </si>
+  <si>
+    <t>Bank_Sys_Design_GUI_Issue_003</t>
+  </si>
+  <si>
+    <t>Bank_Sys_Design_GUI_Issue_004</t>
+  </si>
+  <si>
+    <t>Bank_Sys_Design_GUI_Issue_005</t>
+  </si>
+  <si>
+    <t>Bank_Sys_Design_GUI_Issue_006</t>
+  </si>
+  <si>
+    <t>Bank_Sys_Design_GUI_Issue_007</t>
+  </si>
+  <si>
+    <t>Bank_Sys_Design_GUI_Issue_008</t>
+  </si>
+  <si>
+    <t>Bank_Sys_Design_DM_Issue_001</t>
+  </si>
+  <si>
+    <t>Bank_Sys_Design_DM_Issue_002</t>
+  </si>
+  <si>
+    <t>Bank_Sys_Design_DM_Issue_003</t>
+  </si>
+  <si>
+    <t>Bank_Sys_Design_DM_Issue_004</t>
+  </si>
+  <si>
+    <t>Bank_Sys_Design_DM_Issue_005</t>
+  </si>
+  <si>
+    <t>Bank_Sys_Design_DM_Issue_006</t>
+  </si>
+  <si>
+    <t>Bank_Sys_Design_DM_Issue_007</t>
+  </si>
+  <si>
+    <t>Bank_Sys_Design_DM_Issue_008</t>
+  </si>
+  <si>
+    <t>Bank_Sys_Design_DM_Issue_009</t>
+  </si>
+  <si>
+    <t>Bank_Sys_Design_DM_Issue_010</t>
+  </si>
+  <si>
+    <t>Bank_Sys_Design_DM_Issue_011</t>
+  </si>
+  <si>
+    <t>Bank_Sys_Design_DM_Issue_012</t>
+  </si>
+  <si>
+    <t>Bank_Sys_Design_HLD_Issue_001</t>
+  </si>
+  <si>
+    <t>Bank_Sys_Design_HLD_Issue_002</t>
+  </si>
+  <si>
+    <t>Bank_Sys_Design_HLD_Issue_003</t>
+  </si>
+  <si>
+    <t>Bank_Sys_Design_HLD_Issue_004</t>
+  </si>
+  <si>
+    <t>Bank_Sys_Design_DD_Issue_001</t>
+  </si>
+  <si>
+    <t>Bank_Sys_Design_DD_Issue_002</t>
+  </si>
+  <si>
+    <t>Bank_Sys_Design_DD_Issue_003</t>
+  </si>
+  <si>
+    <t>Bank_Sys_Design_DD_Issue_004</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="14">
     <font>
       <sz val="11"/>
@@ -439,7 +526,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="47">
+  <borders count="44">
     <border>
       <left/>
       <right/>
@@ -672,17 +759,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color theme="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thick">
         <color theme="8"/>
       </left>
@@ -936,30 +1012,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thick">
-        <color theme="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -1020,7 +1072,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1105,28 +1157,28 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1138,43 +1190,43 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1189,13 +1241,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
@@ -1213,19 +1265,10 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1240,13 +1283,13 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1267,44 +1310,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -1315,13 +1325,13 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1330,7 +1340,7 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1339,9 +1349,6 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1354,21 +1361,61 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="標準_REQM_20100521" xfId="1"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="29">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2010,38 +2057,38 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J66"/>
+  <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A47" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="5.77734375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="20.109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="36.77734375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="54.44140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="27.88671875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" style="2" customWidth="1"/>
-    <col min="8" max="10" width="39.88671875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="5.75" style="2" customWidth="1"/>
+    <col min="2" max="2" width="20.125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="32.25" style="5" customWidth="1"/>
+    <col min="4" max="4" width="36.75" style="5" customWidth="1"/>
+    <col min="5" max="5" width="54.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="27.875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="18.125" style="2" customWidth="1"/>
+    <col min="8" max="10" width="39.875" style="2" customWidth="1"/>
     <col min="11" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.4" thickBot="1"/>
+    <row r="1" spans="1:10" ht="15" thickBot="1"/>
     <row r="2" spans="1:10" ht="105" customHeight="1" thickBot="1">
-      <c r="B2" s="98" t="s">
+      <c r="B2" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="100"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
     </row>
     <row r="3" spans="1:10" ht="14.25" customHeight="1">
       <c r="C3" s="7"/>
@@ -2058,26 +2105,26 @@
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:10" ht="20.25" customHeight="1">
-      <c r="C5" s="109" t="s">
+      <c r="C5" s="94" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="109" t="s">
+      <c r="D5" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="111" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="107" t="s">
-        <v>69</v>
-      </c>
-      <c r="G5" s="79"/>
+      <c r="E5" s="96" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="92" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" s="76"/>
     </row>
     <row r="6" spans="1:10" ht="23.25" customHeight="1" thickBot="1">
-      <c r="C6" s="110"/>
-      <c r="D6" s="110"/>
-      <c r="E6" s="112"/>
-      <c r="F6" s="108"/>
-      <c r="G6" s="70"/>
+      <c r="C6" s="95"/>
+      <c r="D6" s="95"/>
+      <c r="E6" s="97"/>
+      <c r="F6" s="93"/>
+      <c r="G6" s="67"/>
     </row>
     <row r="7" spans="1:10" ht="29.25" customHeight="1">
       <c r="C7" s="9">
@@ -2089,53 +2136,53 @@
       <c r="E7" s="57">
         <v>43713</v>
       </c>
-      <c r="F7" s="76" t="s">
-        <v>70</v>
-      </c>
-      <c r="G7" s="70"/>
+      <c r="F7" s="73" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="67"/>
     </row>
     <row r="8" spans="1:10" ht="21.75" customHeight="1">
-      <c r="C8" s="74">
+      <c r="C8" s="71">
         <v>2</v>
       </c>
-      <c r="D8" s="75" t="s">
+      <c r="D8" s="72" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="57">
         <v>43743</v>
       </c>
-      <c r="F8" s="76" t="s">
-        <v>71</v>
-      </c>
-      <c r="G8" s="70"/>
+      <c r="F8" s="73" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" s="67"/>
     </row>
     <row r="9" spans="1:10" ht="21.75" customHeight="1">
       <c r="C9" s="40"/>
       <c r="D9" s="41"/>
       <c r="E9" s="58"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="70"/>
+      <c r="F9" s="69"/>
+      <c r="G9" s="67"/>
     </row>
     <row r="10" spans="1:10" ht="21.75" customHeight="1">
       <c r="C10" s="40"/>
       <c r="D10" s="42"/>
       <c r="E10" s="58"/>
-      <c r="F10" s="71"/>
-      <c r="G10" s="70"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="67"/>
     </row>
     <row r="11" spans="1:10" ht="20.25" customHeight="1">
       <c r="C11" s="40"/>
       <c r="D11" s="43"/>
       <c r="E11" s="58"/>
-      <c r="F11" s="72"/>
-      <c r="G11" s="70"/>
+      <c r="F11" s="69"/>
+      <c r="G11" s="67"/>
     </row>
     <row r="12" spans="1:10" ht="14.25" customHeight="1">
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="70"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="67"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
@@ -2144,8 +2191,8 @@
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
-      <c r="F13" s="70"/>
-      <c r="G13" s="70"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="67"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
@@ -2192,7 +2239,7 @@
         <v>1</v>
       </c>
       <c r="I16" s="60" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="J16" s="63" t="s">
         <v>9</v>
@@ -2200,101 +2247,101 @@
     </row>
     <row r="17" spans="1:10" ht="139.5" customHeight="1" thickTop="1">
       <c r="A17" s="15"/>
-      <c r="B17" s="101" t="s">
+      <c r="B17" s="87" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D17" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="14" t="s">
-        <v>24</v>
-      </c>
       <c r="E17" s="31" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G17" s="30" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H17" s="64" t="s">
-        <v>33</v>
-      </c>
-      <c r="I17" s="89" t="s">
-        <v>65</v>
-      </c>
-      <c r="J17" s="90">
+        <v>27</v>
+      </c>
+      <c r="I17" s="104" t="s">
+        <v>58</v>
+      </c>
+      <c r="J17" s="105">
         <v>43743</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="57" customHeight="1" thickBot="1">
       <c r="A18" s="15"/>
-      <c r="B18" s="96"/>
-      <c r="C18" s="4" t="s">
+      <c r="B18" s="82"/>
+      <c r="C18" s="79" t="s">
+        <v>113</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>26</v>
-      </c>
       <c r="E18" s="8" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F18" s="56" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H18" s="3"/>
-      <c r="I18" s="89"/>
-      <c r="J18" s="91"/>
+      <c r="I18" s="104"/>
+      <c r="J18" s="106"/>
     </row>
     <row r="19" spans="1:10" ht="54.75" customHeight="1">
       <c r="A19" s="15"/>
-      <c r="B19" s="96"/>
-      <c r="C19" s="4" t="s">
+      <c r="B19" s="82"/>
+      <c r="C19" s="79" t="s">
+        <v>114</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="8" t="s">
-        <v>27</v>
-      </c>
       <c r="E19" s="8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H19" s="3"/>
-      <c r="I19" s="89"/>
-      <c r="J19" s="91"/>
+      <c r="I19" s="104"/>
+      <c r="J19" s="106"/>
     </row>
     <row r="20" spans="1:10" s="1" customFormat="1" ht="72.75" customHeight="1" thickBot="1">
       <c r="A20" s="16"/>
-      <c r="B20" s="102"/>
-      <c r="C20" s="26" t="s">
-        <v>22</v>
+      <c r="B20" s="88"/>
+      <c r="C20" s="79" t="s">
+        <v>115</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E20" s="32" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F20" s="32" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G20" s="26" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H20" s="19"/>
-      <c r="I20" s="89"/>
-      <c r="J20" s="91"/>
-    </row>
-    <row r="21" spans="1:10" s="6" customFormat="1" ht="4.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="I20" s="104"/>
+      <c r="J20" s="106"/>
+    </row>
+    <row r="21" spans="1:10" s="6" customFormat="1" ht="18" customHeight="1" thickTop="1" thickBot="1">
       <c r="A21" s="17"/>
       <c r="B21" s="25"/>
       <c r="C21" s="35"/>
@@ -2308,107 +2355,141 @@
     </row>
     <row r="22" spans="1:10" ht="57" customHeight="1" thickTop="1">
       <c r="A22" s="15"/>
-      <c r="B22" s="103" t="s">
+      <c r="B22" s="89" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="14"/>
+      <c r="C22" s="79" t="s">
+        <v>116</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>85</v>
+      </c>
       <c r="E22" s="14" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="F22" s="14"/>
-      <c r="G22" s="13"/>
+      <c r="G22" s="13" t="s">
+        <v>17</v>
+      </c>
       <c r="H22" s="30"/>
-      <c r="I22" s="92" t="s">
-        <v>66</v>
-      </c>
-      <c r="J22" s="93">
+      <c r="I22" s="107" t="s">
+        <v>59</v>
+      </c>
+      <c r="J22" s="108">
         <v>43743</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="54.75" customHeight="1">
+    <row r="23" spans="1:10" ht="54.75" customHeight="1" thickBot="1">
       <c r="A23" s="15"/>
-      <c r="B23" s="104"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
+      <c r="B23" s="90"/>
+      <c r="C23" s="79" t="s">
+        <v>117</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>86</v>
+      </c>
       <c r="F23" s="8"/>
-      <c r="G23" s="4"/>
+      <c r="G23" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H23" s="4"/>
-      <c r="I23" s="92"/>
-      <c r="J23" s="94"/>
-    </row>
-    <row r="24" spans="1:10" ht="60" customHeight="1">
+      <c r="I23" s="107"/>
+      <c r="J23" s="109"/>
+    </row>
+    <row r="24" spans="1:10" ht="89.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A24" s="15"/>
-      <c r="B24" s="104"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
+      <c r="B24" s="90"/>
+      <c r="C24" s="79" t="s">
+        <v>118</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>87</v>
+      </c>
       <c r="F24" s="8"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="92"/>
-      <c r="J24" s="94"/>
-    </row>
-    <row r="25" spans="1:10" ht="60" customHeight="1">
+      <c r="G24" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H24" s="64" t="s">
+        <v>89</v>
+      </c>
+      <c r="I24" s="107"/>
+      <c r="J24" s="109"/>
+    </row>
+    <row r="25" spans="1:10" ht="88.5" customHeight="1" thickTop="1">
       <c r="A25" s="15"/>
-      <c r="B25" s="104"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
+      <c r="B25" s="90"/>
+      <c r="C25" s="79" t="s">
+        <v>119</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E25" s="32" t="s">
+        <v>88</v>
+      </c>
       <c r="F25" s="32"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="92"/>
-      <c r="J25" s="94"/>
+      <c r="G25" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="H25" s="64" t="s">
+        <v>90</v>
+      </c>
+      <c r="I25" s="107"/>
+      <c r="J25" s="109"/>
     </row>
     <row r="26" spans="1:10" ht="60" customHeight="1">
       <c r="A26" s="15"/>
-      <c r="B26" s="104"/>
+      <c r="B26" s="90"/>
       <c r="C26" s="26"/>
       <c r="D26" s="32"/>
       <c r="E26" s="32"/>
       <c r="F26" s="32"/>
-      <c r="G26" s="26"/>
+      <c r="G26" s="78"/>
       <c r="H26" s="26"/>
-      <c r="I26" s="92"/>
-      <c r="J26" s="94"/>
+      <c r="I26" s="107"/>
+      <c r="J26" s="109"/>
     </row>
     <row r="27" spans="1:10" ht="60" customHeight="1">
       <c r="A27" s="15"/>
-      <c r="B27" s="104"/>
+      <c r="B27" s="90"/>
       <c r="C27" s="26"/>
       <c r="D27" s="32"/>
       <c r="E27" s="32"/>
       <c r="F27" s="32"/>
       <c r="G27" s="26"/>
       <c r="H27" s="26"/>
-      <c r="I27" s="92"/>
-      <c r="J27" s="94"/>
+      <c r="I27" s="107"/>
+      <c r="J27" s="109"/>
     </row>
     <row r="28" spans="1:10" ht="60" customHeight="1">
       <c r="A28" s="15"/>
-      <c r="B28" s="104"/>
+      <c r="B28" s="90"/>
       <c r="C28" s="26"/>
       <c r="D28" s="32"/>
       <c r="E28" s="32"/>
       <c r="F28" s="32"/>
       <c r="G28" s="26"/>
       <c r="H28" s="26"/>
-      <c r="I28" s="92"/>
-      <c r="J28" s="94"/>
+      <c r="I28" s="107"/>
+      <c r="J28" s="109"/>
     </row>
     <row r="29" spans="1:10" ht="51.75" customHeight="1" thickBot="1">
       <c r="A29" s="15"/>
-      <c r="B29" s="105"/>
+      <c r="B29" s="91"/>
       <c r="C29" s="26"/>
       <c r="D29" s="32"/>
       <c r="E29" s="32"/>
       <c r="F29" s="32"/>
       <c r="G29" s="26"/>
       <c r="H29" s="18"/>
-      <c r="I29" s="92"/>
-      <c r="J29" s="94"/>
+      <c r="I29" s="107"/>
+      <c r="J29" s="109"/>
     </row>
     <row r="30" spans="1:10" ht="5.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A30" s="15"/>
@@ -2424,281 +2505,305 @@
     </row>
     <row r="31" spans="1:10" ht="71.25" customHeight="1" thickTop="1">
       <c r="A31" s="15"/>
-      <c r="B31" s="96" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" s="13"/>
+      <c r="B31" s="82" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" s="79" t="s">
+        <v>100</v>
+      </c>
       <c r="D31" s="14" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F31" s="14" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="G31" s="13" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H31" s="65"/>
-      <c r="I31" s="92" t="s">
-        <v>67</v>
-      </c>
-      <c r="J31" s="93">
+      <c r="I31" s="107" t="s">
+        <v>60</v>
+      </c>
+      <c r="J31" s="108">
         <v>43743</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="63" customHeight="1">
       <c r="A32" s="15"/>
-      <c r="B32" s="96"/>
-      <c r="C32" s="4"/>
+      <c r="B32" s="82"/>
+      <c r="C32" s="79" t="s">
+        <v>101</v>
+      </c>
       <c r="D32" s="4" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="H32" s="3"/>
-      <c r="I32" s="92"/>
-      <c r="J32" s="94"/>
+      <c r="I32" s="107"/>
+      <c r="J32" s="109"/>
     </row>
     <row r="33" spans="1:10" ht="62.25" customHeight="1">
       <c r="A33" s="15"/>
-      <c r="B33" s="96"/>
-      <c r="C33" s="4"/>
+      <c r="B33" s="82"/>
+      <c r="C33" s="79" t="s">
+        <v>102</v>
+      </c>
       <c r="D33" s="4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H33" s="3"/>
-      <c r="I33" s="92"/>
-      <c r="J33" s="94"/>
+      <c r="I33" s="107"/>
+      <c r="J33" s="109"/>
     </row>
     <row r="34" spans="1:10" ht="62.25" customHeight="1">
       <c r="A34" s="15"/>
-      <c r="B34" s="96"/>
-      <c r="C34" s="26"/>
+      <c r="B34" s="82"/>
+      <c r="C34" s="79" t="s">
+        <v>103</v>
+      </c>
       <c r="D34" s="26" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E34" s="27" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F34" s="32"/>
       <c r="G34" s="26" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H34" s="27"/>
-      <c r="I34" s="92"/>
-      <c r="J34" s="94"/>
+      <c r="I34" s="107"/>
+      <c r="J34" s="109"/>
     </row>
     <row r="35" spans="1:10" ht="62.25" customHeight="1">
       <c r="A35" s="15"/>
-      <c r="B35" s="96"/>
-      <c r="C35" s="26"/>
+      <c r="B35" s="82"/>
+      <c r="C35" s="79" t="s">
+        <v>104</v>
+      </c>
       <c r="D35" s="26" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E35" s="55" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="F35" s="32" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G35" s="26" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H35" s="27"/>
-      <c r="I35" s="92"/>
-      <c r="J35" s="94"/>
+      <c r="I35" s="107"/>
+      <c r="J35" s="109"/>
     </row>
     <row r="36" spans="1:10" ht="62.25" customHeight="1">
       <c r="A36" s="15"/>
-      <c r="B36" s="96"/>
-      <c r="C36" s="26"/>
+      <c r="B36" s="82"/>
+      <c r="C36" s="79" t="s">
+        <v>105</v>
+      </c>
       <c r="D36" s="26" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="E36" s="55" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="F36" s="32" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G36" s="26" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H36" s="27"/>
-      <c r="I36" s="92"/>
-      <c r="J36" s="94"/>
+      <c r="I36" s="107"/>
+      <c r="J36" s="109"/>
     </row>
     <row r="37" spans="1:10" ht="62.25" customHeight="1">
       <c r="A37" s="15"/>
-      <c r="B37" s="96"/>
-      <c r="C37" s="26"/>
+      <c r="B37" s="82"/>
+      <c r="C37" s="79" t="s">
+        <v>106</v>
+      </c>
       <c r="D37" s="26" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E37" s="55" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="F37" s="32" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="G37" s="26" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="H37" s="27"/>
-      <c r="I37" s="92"/>
-      <c r="J37" s="94"/>
+      <c r="I37" s="107"/>
+      <c r="J37" s="109"/>
     </row>
     <row r="38" spans="1:10" ht="62.25" customHeight="1">
       <c r="A38" s="15"/>
-      <c r="B38" s="96"/>
-      <c r="C38" s="26"/>
+      <c r="B38" s="82"/>
+      <c r="C38" s="79" t="s">
+        <v>107</v>
+      </c>
       <c r="D38" s="26" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E38" s="55" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="F38" s="32" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="G38" s="26" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H38" s="27"/>
-      <c r="I38" s="92"/>
-      <c r="J38" s="94"/>
+      <c r="I38" s="107"/>
+      <c r="J38" s="109"/>
     </row>
     <row r="39" spans="1:10" ht="62.25" customHeight="1">
       <c r="A39" s="15"/>
-      <c r="B39" s="96"/>
-      <c r="C39" s="26"/>
+      <c r="B39" s="82"/>
+      <c r="C39" s="79" t="s">
+        <v>108</v>
+      </c>
       <c r="D39" s="26" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E39" s="55" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F39" s="32" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="G39" s="26" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H39" s="27"/>
-      <c r="I39" s="92"/>
-      <c r="J39" s="94"/>
+      <c r="I39" s="107"/>
+      <c r="J39" s="109"/>
     </row>
     <row r="40" spans="1:10" ht="62.25" customHeight="1">
       <c r="A40" s="15"/>
-      <c r="B40" s="96"/>
-      <c r="C40" s="26"/>
+      <c r="B40" s="82"/>
+      <c r="C40" s="79" t="s">
+        <v>109</v>
+      </c>
       <c r="D40" s="26" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E40" s="55" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F40" s="32" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="G40" s="26" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H40" s="27"/>
-      <c r="I40" s="92"/>
-      <c r="J40" s="94"/>
+      <c r="I40" s="107"/>
+      <c r="J40" s="109"/>
     </row>
     <row r="41" spans="1:10" ht="62.25" customHeight="1">
       <c r="A41" s="15"/>
-      <c r="B41" s="96"/>
-      <c r="C41" s="26"/>
+      <c r="B41" s="82"/>
+      <c r="C41" s="79" t="s">
+        <v>110</v>
+      </c>
       <c r="D41" s="26" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E41" s="55" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F41" s="32" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="G41" s="26" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="H41" s="27"/>
-      <c r="I41" s="92"/>
-      <c r="J41" s="94"/>
+      <c r="I41" s="107"/>
+      <c r="J41" s="109"/>
     </row>
     <row r="42" spans="1:10" ht="62.25" customHeight="1">
       <c r="A42" s="15"/>
-      <c r="B42" s="96"/>
-      <c r="C42" s="26"/>
+      <c r="B42" s="82"/>
+      <c r="C42" s="79" t="s">
+        <v>111</v>
+      </c>
       <c r="D42" s="26" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E42" s="55" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F42" s="32"/>
       <c r="G42" s="26" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H42" s="27"/>
-      <c r="I42" s="92"/>
-      <c r="J42" s="94"/>
+      <c r="I42" s="107"/>
+      <c r="J42" s="109"/>
     </row>
     <row r="43" spans="1:10" ht="62.25" customHeight="1">
       <c r="A43" s="15"/>
-      <c r="B43" s="96"/>
+      <c r="B43" s="82"/>
       <c r="C43" s="26"/>
       <c r="D43" s="26"/>
       <c r="E43" s="55"/>
       <c r="F43" s="32"/>
       <c r="G43" s="26"/>
       <c r="H43" s="27"/>
-      <c r="I43" s="92"/>
-      <c r="J43" s="94"/>
+      <c r="I43" s="107"/>
+      <c r="J43" s="109"/>
     </row>
     <row r="44" spans="1:10" ht="62.25" customHeight="1">
       <c r="A44" s="15"/>
-      <c r="B44" s="96"/>
+      <c r="B44" s="82"/>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
       <c r="E44" s="55"/>
       <c r="F44" s="32"/>
       <c r="G44" s="26"/>
       <c r="H44" s="27"/>
-      <c r="I44" s="92"/>
-      <c r="J44" s="94"/>
+      <c r="I44" s="107"/>
+      <c r="J44" s="109"/>
     </row>
     <row r="45" spans="1:10" ht="62.25" customHeight="1" thickBot="1">
       <c r="A45" s="15"/>
-      <c r="B45" s="96"/>
+      <c r="B45" s="82"/>
       <c r="C45" s="26"/>
       <c r="D45" s="26"/>
       <c r="E45" s="55"/>
       <c r="F45" s="32"/>
       <c r="G45" s="26"/>
       <c r="H45" s="19"/>
-      <c r="I45" s="92"/>
-      <c r="J45" s="94"/>
+      <c r="I45" s="107"/>
+      <c r="J45" s="109"/>
     </row>
     <row r="46" spans="1:10" ht="6.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A46" s="15"/>
@@ -2712,7 +2817,7 @@
       <c r="I46" s="52"/>
       <c r="J46" s="54"/>
     </row>
-    <row r="47" spans="1:10" ht="6.75" customHeight="1" thickTop="1">
+    <row r="47" spans="1:10" ht="6.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A47" s="50"/>
       <c r="B47" s="51"/>
       <c r="C47" s="52"/>
@@ -2724,224 +2829,207 @@
       <c r="I47" s="52"/>
       <c r="J47" s="54"/>
     </row>
-    <row r="48" spans="1:10" ht="58.5" customHeight="1">
-      <c r="B48" s="96" t="s">
-        <v>15</v>
-      </c>
-      <c r="C48" s="13"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="13"/>
-      <c r="H48" s="66"/>
-      <c r="I48" s="81" t="s">
+    <row r="48" spans="1:10" ht="6.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A48" s="15"/>
+      <c r="B48" s="28"/>
+      <c r="C48" s="35"/>
+      <c r="D48" s="33"/>
+      <c r="E48" s="34"/>
+      <c r="F48" s="39"/>
+      <c r="G48" s="35"/>
+      <c r="H48" s="36"/>
+      <c r="I48" s="52"/>
+      <c r="J48" s="52"/>
+    </row>
+    <row r="49" spans="1:10" ht="137.44999999999999" customHeight="1" thickTop="1">
+      <c r="A49" s="15"/>
+      <c r="B49" s="81" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49" s="79" t="s">
+        <v>92</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E49" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="F49" s="14"/>
+      <c r="G49" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H49" s="65"/>
+      <c r="I49" s="100" t="s">
+        <v>61</v>
+      </c>
+      <c r="J49" s="102">
+        <v>43743</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="45" customHeight="1">
+      <c r="A50" s="50"/>
+      <c r="B50" s="81"/>
+      <c r="C50" s="79" t="s">
+        <v>93</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E50" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="J48" s="84"/>
-    </row>
-    <row r="49" spans="1:10" ht="48.75" customHeight="1">
-      <c r="B49" s="96"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="8"/>
-      <c r="F49" s="8"/>
-      <c r="G49" s="4"/>
-      <c r="H49" s="67"/>
-      <c r="I49" s="82"/>
-      <c r="J49" s="84"/>
-    </row>
-    <row r="50" spans="1:10" ht="51.75" customHeight="1">
-      <c r="B50" s="96"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="4"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="8"/>
-      <c r="G50" s="4"/>
-      <c r="H50" s="67"/>
-      <c r="I50" s="82"/>
-      <c r="J50" s="84"/>
-    </row>
-    <row r="51" spans="1:10" ht="45.75" customHeight="1" thickBot="1">
-      <c r="A51" s="15"/>
-      <c r="B51" s="106"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="18"/>
-      <c r="G51" s="18"/>
-      <c r="H51" s="68"/>
-      <c r="I51" s="83"/>
-      <c r="J51" s="84"/>
-    </row>
-    <row r="52" spans="1:10" ht="6.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A52" s="15"/>
-      <c r="B52" s="28"/>
-      <c r="C52" s="35"/>
-      <c r="D52" s="33"/>
-      <c r="E52" s="34"/>
-      <c r="F52" s="39"/>
-      <c r="G52" s="35"/>
-      <c r="H52" s="36"/>
-      <c r="I52" s="52"/>
-      <c r="J52" s="52"/>
-    </row>
-    <row r="53" spans="1:10" ht="137.4" customHeight="1" thickTop="1">
-      <c r="A53" s="15"/>
-      <c r="B53" s="95" t="s">
-        <v>16</v>
-      </c>
-      <c r="C53" s="13"/>
-      <c r="D53" s="14" t="s">
+      <c r="F50" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="G50" s="75" t="s">
+        <v>17</v>
+      </c>
+      <c r="H50" s="77"/>
+      <c r="I50" s="98"/>
+      <c r="J50" s="99"/>
+    </row>
+    <row r="51" spans="1:10" ht="45.75" customHeight="1">
+      <c r="B51" s="82"/>
+      <c r="C51" s="79" t="s">
+        <v>94</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F51" s="8"/>
+      <c r="G51" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H51" s="3"/>
+      <c r="I51" s="98"/>
+      <c r="J51" s="99"/>
+    </row>
+    <row r="52" spans="1:10" ht="45.75" customHeight="1">
+      <c r="B52" s="82"/>
+      <c r="C52" s="79" t="s">
+        <v>95</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F52" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="E53" s="14" t="s">
+      <c r="G52" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H52" s="3"/>
+      <c r="I52" s="98"/>
+      <c r="J52" s="99"/>
+    </row>
+    <row r="53" spans="1:10" ht="45" customHeight="1">
+      <c r="B53" s="82"/>
+      <c r="C53" s="79" t="s">
+        <v>96</v>
+      </c>
+      <c r="D53" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F53" s="14"/>
-      <c r="G53" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="H53" s="65"/>
-      <c r="I53" s="85" t="s">
-        <v>68</v>
-      </c>
-      <c r="J53" s="87">
-        <v>43743</v>
-      </c>
+      <c r="E53" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H53" s="3"/>
+      <c r="I53" s="98"/>
+      <c r="J53" s="99"/>
     </row>
     <row r="54" spans="1:10" ht="45" customHeight="1">
-      <c r="A54" s="50"/>
-      <c r="B54" s="95"/>
-      <c r="C54" s="78"/>
-      <c r="D54" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E54" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="F54" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="G54" s="78" t="s">
-        <v>23</v>
-      </c>
-      <c r="H54" s="80"/>
-      <c r="I54" s="82"/>
-      <c r="J54" s="84"/>
-    </row>
-    <row r="55" spans="1:10" ht="45.75" customHeight="1">
-      <c r="B55" s="96"/>
-      <c r="C55" s="4"/>
-      <c r="D55" s="4" t="s">
+      <c r="B54" s="82"/>
+      <c r="C54" s="79" t="s">
+        <v>97</v>
+      </c>
+      <c r="D54" s="74" t="s">
         <v>77</v>
       </c>
-      <c r="E55" s="8" t="s">
+      <c r="E54" s="55" t="s">
         <v>76</v>
       </c>
-      <c r="F55" s="8"/>
-      <c r="G55" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H55" s="3"/>
-      <c r="I55" s="82"/>
-      <c r="J55" s="84"/>
-    </row>
-    <row r="56" spans="1:10" ht="45.75" customHeight="1">
-      <c r="B56" s="96"/>
-      <c r="C56" s="4"/>
-      <c r="D56" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E56" s="8" t="s">
+      <c r="F54" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="F56" s="8" t="s">
+      <c r="G54" s="74" t="s">
+        <v>34</v>
+      </c>
+      <c r="H54" s="27"/>
+      <c r="I54" s="98"/>
+      <c r="J54" s="99"/>
+    </row>
+    <row r="55" spans="1:10" ht="45" customHeight="1">
+      <c r="B55" s="82"/>
+      <c r="C55" s="79" t="s">
+        <v>98</v>
+      </c>
+      <c r="D55" s="74" t="s">
+        <v>80</v>
+      </c>
+      <c r="E55" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="G56" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H56" s="3"/>
-      <c r="I56" s="82"/>
-      <c r="J56" s="84"/>
-    </row>
-    <row r="57" spans="1:10" ht="45" customHeight="1">
-      <c r="B57" s="96"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E57" s="8" t="s">
+      <c r="F55" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G55" s="74" t="s">
+        <v>34</v>
+      </c>
+      <c r="H55" s="27"/>
+      <c r="I55" s="98"/>
+      <c r="J55" s="99"/>
+    </row>
+    <row r="56" spans="1:10" ht="44.25" customHeight="1" thickBot="1">
+      <c r="B56" s="83"/>
+      <c r="C56" s="79" t="s">
+        <v>99</v>
+      </c>
+      <c r="D56" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="E56" s="80" t="s">
         <v>81</v>
       </c>
-      <c r="F57" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="G57" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H57" s="3"/>
-      <c r="I57" s="82"/>
-      <c r="J57" s="84"/>
-    </row>
-    <row r="58" spans="1:10" ht="45" customHeight="1">
-      <c r="B58" s="96"/>
-      <c r="C58" s="77"/>
-      <c r="D58" s="77" t="s">
-        <v>84</v>
-      </c>
-      <c r="E58" s="55" t="s">
+      <c r="F56" s="80" t="s">
         <v>83</v>
       </c>
-      <c r="F58" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="G58" s="77" t="s">
-        <v>40</v>
-      </c>
-      <c r="H58" s="27"/>
-      <c r="I58" s="82"/>
-      <c r="J58" s="84"/>
-    </row>
-    <row r="59" spans="1:10" ht="45" customHeight="1">
-      <c r="B59" s="96"/>
-      <c r="C59" s="77"/>
-      <c r="D59" s="77" t="s">
-        <v>87</v>
-      </c>
-      <c r="E59" s="32" t="s">
-        <v>86</v>
-      </c>
-      <c r="F59" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="G59" s="77" t="s">
-        <v>40</v>
-      </c>
-      <c r="H59" s="27"/>
-      <c r="I59" s="82"/>
-      <c r="J59" s="84"/>
-    </row>
-    <row r="60" spans="1:10" ht="44.25" customHeight="1" thickBot="1">
-      <c r="B60" s="97"/>
-      <c r="C60" s="18"/>
-      <c r="D60" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="E60" s="113" t="s">
-        <v>88</v>
-      </c>
-      <c r="F60" s="113" t="s">
-        <v>90</v>
-      </c>
-      <c r="G60" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="H60" s="19"/>
-      <c r="I60" s="86"/>
-      <c r="J60" s="88"/>
-    </row>
-    <row r="61" spans="1:10" ht="14.4" thickTop="1">
+      <c r="G56" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H56" s="19"/>
+      <c r="I56" s="101"/>
+      <c r="J56" s="103"/>
+    </row>
+    <row r="57" spans="1:10" ht="15" thickTop="1">
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+    </row>
+    <row r="61" spans="1:10">
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
     </row>
@@ -2949,176 +3037,149 @@
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
     </row>
-    <row r="63" spans="1:10">
-      <c r="C63" s="2"/>
-      <c r="D63" s="2"/>
-    </row>
-    <row r="64" spans="1:10">
-      <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
-    </row>
-    <row r="65" spans="3:4">
-      <c r="C65" s="2"/>
-      <c r="D65" s="2"/>
-    </row>
-    <row r="66" spans="3:4">
-      <c r="C66" s="2"/>
-      <c r="D66" s="2"/>
-    </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="B53:B60"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="B22:B29"/>
-    <mergeCell ref="B48:B51"/>
-    <mergeCell ref="B31:B45"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="I48:I51"/>
-    <mergeCell ref="J48:J51"/>
-    <mergeCell ref="I53:I60"/>
-    <mergeCell ref="J53:J60"/>
+  <mergeCells count="17">
+    <mergeCell ref="I49:I56"/>
+    <mergeCell ref="J49:J56"/>
     <mergeCell ref="I17:I20"/>
     <mergeCell ref="J17:J20"/>
     <mergeCell ref="I22:I29"/>
     <mergeCell ref="J22:J29"/>
     <mergeCell ref="I31:I45"/>
     <mergeCell ref="J31:J45"/>
+    <mergeCell ref="B49:B56"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="B22:B29"/>
+    <mergeCell ref="B31:B45"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
-  <conditionalFormatting sqref="C33:E45 G32:H45 C32:D32 H22:J22 H30:J31 H23:H29 C60:E60 C59:D59">
-    <cfRule type="expression" dxfId="27" priority="28" stopIfTrue="1">
+  <conditionalFormatting sqref="C43:E45 G32:H45 D32 H22:J22 H30:J31 H23 D56:E56 D55 H26:H29 D33:E42">
+    <cfRule type="expression" dxfId="28" priority="32" stopIfTrue="1">
       <formula>$H22="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E22:E32 C22:D31 G22:G31 C17:J17 C21:J21 C18:E18 G18:H18 C19:H20">
-    <cfRule type="expression" dxfId="26" priority="33" stopIfTrue="1">
+  <conditionalFormatting sqref="E22:E32 C17:J17 C21:J21 D18:E18 G18:H18 D19:H20 G22:G31 C26:D31 C32:C42 C18:C20 C22:C25">
+    <cfRule type="expression" dxfId="27" priority="37" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22:F29 F32:F45">
-    <cfRule type="expression" dxfId="25" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="27" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F30">
-    <cfRule type="expression" dxfId="24" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="26" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F31">
-    <cfRule type="expression" dxfId="23" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="25" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50:E51 G49:H51 C49:D49 H48:J48">
-    <cfRule type="expression" dxfId="22" priority="19" stopIfTrue="1">
+  <conditionalFormatting sqref="H46:J47">
+    <cfRule type="expression" dxfId="18" priority="18" stopIfTrue="1">
+      <formula>$H46="close"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C46:E47 G46:G47">
+    <cfRule type="expression" dxfId="17" priority="19" stopIfTrue="1">
+      <formula>#REF!="close"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F46:F47">
+    <cfRule type="expression" dxfId="16" priority="17" stopIfTrue="1">
+      <formula>#REF!="close"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H48:J48">
+    <cfRule type="expression" dxfId="15" priority="15" stopIfTrue="1">
       <formula>$H48="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F51">
-    <cfRule type="expression" dxfId="21" priority="18" stopIfTrue="1">
-      <formula>$H51="close"</formula>
+  <conditionalFormatting sqref="C48:E48 G48">
+    <cfRule type="expression" dxfId="14" priority="16" stopIfTrue="1">
+      <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E48:E49 C48:D48 G48">
-    <cfRule type="expression" dxfId="20" priority="20" stopIfTrue="1">
+  <conditionalFormatting sqref="F48">
+    <cfRule type="expression" dxfId="13" priority="14" stopIfTrue="1">
+      <formula>#REF!="close"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D53:E53 G51:H56 D51:D52 H49:J50 D54">
+    <cfRule type="expression" dxfId="12" priority="12" stopIfTrue="1">
+      <formula>$H49="close"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E49:E52 D50 G49:G50">
+    <cfRule type="expression" dxfId="11" priority="13" stopIfTrue="1">
+      <formula>#REF!="close"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F51:F53">
+    <cfRule type="expression" dxfId="10" priority="10" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F49:F50">
-    <cfRule type="expression" dxfId="19" priority="17" stopIfTrue="1">
-      <formula>#REF!="close"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F48">
-    <cfRule type="expression" dxfId="18" priority="16" stopIfTrue="1">
-      <formula>#REF!="close"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H46:J47">
-    <cfRule type="expression" dxfId="17" priority="14" stopIfTrue="1">
-      <formula>$H46="close"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C46:E47 G46:G47">
-    <cfRule type="expression" dxfId="16" priority="15" stopIfTrue="1">
-      <formula>#REF!="close"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F46:F47">
-    <cfRule type="expression" dxfId="15" priority="13" stopIfTrue="1">
-      <formula>#REF!="close"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H52:J52">
-    <cfRule type="expression" dxfId="14" priority="11" stopIfTrue="1">
-      <formula>$H52="close"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C52:E52 G52">
-    <cfRule type="expression" dxfId="13" priority="12" stopIfTrue="1">
-      <formula>#REF!="close"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F52">
-    <cfRule type="expression" dxfId="12" priority="10" stopIfTrue="1">
-      <formula>#REF!="close"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57:E57 G55:H60 C55:D56 H53:J54 C58:D58">
-    <cfRule type="expression" dxfId="11" priority="8" stopIfTrue="1">
-      <formula>$H53="close"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E53:E56 C54:D54 G53:G54 C53">
     <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F55:F57">
-    <cfRule type="expression" dxfId="8" priority="6" stopIfTrue="1">
+  <conditionalFormatting sqref="E54">
+    <cfRule type="expression" dxfId="8" priority="39" stopIfTrue="1">
+      <formula>$H55="close"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E55">
+    <cfRule type="expression" dxfId="7" priority="8" stopIfTrue="1">
+      <formula>$H55="close"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F54:F55">
+    <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F53:F54">
-    <cfRule type="expression" dxfId="7" priority="5" stopIfTrue="1">
+  <conditionalFormatting sqref="F56">
+    <cfRule type="expression" dxfId="5" priority="6" stopIfTrue="1">
+      <formula>$H56="close"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D49">
+    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E58">
-    <cfRule type="expression" dxfId="6" priority="35" stopIfTrue="1">
-      <formula>$H59="close"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E59">
-    <cfRule type="expression" dxfId="5" priority="4" stopIfTrue="1">
-      <formula>$H59="close"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F58:F59">
-    <cfRule type="expression" dxfId="4" priority="3" stopIfTrue="1">
+  <conditionalFormatting sqref="D22:D25">
+    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F60">
-    <cfRule type="expression" dxfId="3" priority="2" stopIfTrue="1">
-      <formula>$H60="close"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D53">
-    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+  <conditionalFormatting sqref="H24">
+    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
       <formula>#REF!="close"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F51">
-      <formula1>"Organizational,Technical, Business ,Product"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H22:H60">
+  <conditionalFormatting sqref="H25">
+    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+      <formula>#REF!="close"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C56">
+    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+      <formula>#REF!="close"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H22:H23 H26:H56">
       <formula1>"close,open"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>